<commit_message>
mouse wheel scrolling, page up, page down
</commit_message>
<xml_diff>
--- a/Feature Matrix.xlsx
+++ b/Feature Matrix.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="175">
   <si>
     <t>Feature</t>
   </si>
@@ -449,12 +449,6 @@
     <t>scroll wheel</t>
   </si>
   <si>
-    <t>keyboard modifier keys ignored</t>
-  </si>
-  <si>
-    <t>scrolls the viewport</t>
-  </si>
-  <si>
     <t>replaces selection</t>
   </si>
   <si>
@@ -540,6 +534,15 @@
   </si>
   <si>
     <t>scrolls to visible when dragging outside of the component boundaries</t>
+  </si>
+  <si>
+    <t>block scroll up</t>
+  </si>
+  <si>
+    <t>block scroll down</t>
+  </si>
+  <si>
+    <t>ctrl-scroll wheel</t>
   </si>
 </sst>
 </file>
@@ -797,8 +800,8 @@
           <c:yMode val="edge"/>
           <c:x val="3.8461559098965002E-2"/>
           <c:y val="2.2690437601296611E-2"/>
-          <c:w val="0.9197807133095498"/>
-          <c:h val="0.89627228525119962"/>
+          <c:w val="0.91978071330954991"/>
+          <c:h val="0.89627228525119951"/>
         </c:manualLayout>
       </c:layout>
       <c:areaChart>
@@ -830,10 +833,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Progress!$A$48:$A$51</c:f>
+              <c:f>Progress!$A$48:$A$52</c:f>
               <c:numCache>
                 <c:formatCode>[$-409]mmmm\ d\,\ yyyy;@</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>42699</c:v>
                 </c:pt>
@@ -846,15 +849,18 @@
                 <c:pt idx="3">
                   <c:v>42847</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>42855</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Progress!$B$48:$B$51</c:f>
+              <c:f>Progress!$B$48:$B$52</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -866,6 +872,9 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>42</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -898,10 +907,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Progress!$A$48:$A$51</c:f>
+              <c:f>Progress!$A$48:$A$52</c:f>
               <c:numCache>
                 <c:formatCode>[$-409]mmmm\ d\,\ yyyy;@</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>42699</c:v>
                 </c:pt>
@@ -914,15 +923,18 @@
                 <c:pt idx="3">
                   <c:v>42847</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>42855</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Progress!$C$48:$C$51</c:f>
+              <c:f>Progress!$C$48:$C$52</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -934,6 +946,9 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>126</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>119</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -966,10 +981,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Progress!$A$48:$A$51</c:f>
+              <c:f>Progress!$A$48:$A$52</c:f>
               <c:numCache>
                 <c:formatCode>[$-409]mmmm\ d\,\ yyyy;@</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>42699</c:v>
                 </c:pt>
@@ -982,15 +997,18 @@
                 <c:pt idx="3">
                   <c:v>42847</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>42855</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Progress!$D$48:$D$51</c:f>
+              <c:f>Progress!$D$48:$D$52</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1001,6 +1019,9 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
@@ -1034,10 +1055,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Progress!$A$48:$A$51</c:f>
+              <c:f>Progress!$A$48:$A$52</c:f>
               <c:numCache>
                 <c:formatCode>[$-409]mmmm\ d\,\ yyyy;@</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>42699</c:v>
                 </c:pt>
@@ -1050,15 +1071,18 @@
                 <c:pt idx="3">
                   <c:v>42847</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>42855</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Progress!$E$48:$E$55</c:f>
+              <c:f>Progress!$E$48:$E$56</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1071,21 +1095,24 @@
                 <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="122211712"/>
-        <c:axId val="121967744"/>
+        <c:axId val="133090688"/>
+        <c:axId val="132781184"/>
       </c:areaChart>
       <c:dateAx>
-        <c:axId val="122211712"/>
+        <c:axId val="133090688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1118,7 +1145,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="121967744"/>
+        <c:crossAx val="132781184"/>
         <c:crosses val="autoZero"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
@@ -1128,7 +1155,7 @@
         <c:minorTimeUnit val="months"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="121967744"/>
+        <c:axId val="132781184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1170,7 +1197,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="122211712"/>
+        <c:crossAx val="133090688"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1192,8 +1219,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="4.582822980460776E-2"/>
-          <c:y val="0.3381955699621827"/>
+          <c:x val="4.5828229804607774E-2"/>
+          <c:y val="0.33819556996218281"/>
           <c:w val="0.12857154394162268"/>
           <c:h val="0.11669367909238262"/>
         </c:manualLayout>
@@ -1260,7 +1287,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="1" l="0.75000000000001199" r="0.75000000000001199" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.7500000000000121" r="0.7500000000000121" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup paperSize="9" orientation="landscape" horizontalDpi="1200" verticalDpi="1200"/>
   </c:printSettings>
 </c:chartSpace>
@@ -1314,7 +1341,7 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="4.4510450248127331E-2"/>
+          <c:x val="4.4510450248127345E-2"/>
           <c:y val="0.10032394165889739"/>
           <c:w val="0.79228601441663349"/>
           <c:h val="0.79935527708863363"/>
@@ -1349,10 +1376,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Progress!$A$48:$A$51</c:f>
+              <c:f>Progress!$A$48:$A$52</c:f>
               <c:numCache>
                 <c:formatCode>[$-409]mmmm\ d\,\ yyyy;@</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>42699</c:v>
                 </c:pt>
@@ -1365,15 +1392,18 @@
                 <c:pt idx="3">
                   <c:v>42847</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>42855</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Progress!$G$48:$G$51</c:f>
+              <c:f>Progress!$G$48:$G$52</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1386,15 +1416,18 @@
                 <c:pt idx="3">
                   <c:v>0.2</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.25766871165644173</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="122012032"/>
-        <c:axId val="122013568"/>
+        <c:axId val="132817280"/>
+        <c:axId val="132818816"/>
       </c:areaChart>
       <c:dateAx>
-        <c:axId val="122012032"/>
+        <c:axId val="132817280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1402,13 +1435,13 @@
         <c:axPos val="b"/>
         <c:numFmt formatCode="[$-409]mmmm\ d\,\ yyyy;@" sourceLinked="1"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="122013568"/>
+        <c:crossAx val="132818816"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="122013568"/>
+        <c:axId val="132818816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1451,7 +1484,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="122012032"/>
+        <c:crossAx val="132817280"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1500,7 +1533,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="1" l="0.75000000000001199" r="0.75000000000001199" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.7500000000000121" r="0.7500000000000121" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
   </c:printSettings>
 </c:chartSpace>
@@ -1551,10 +1584,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Progress!$A$48:$A$51</c:f>
+              <c:f>Progress!$A$48:$A$52</c:f>
               <c:numCache>
                 <c:formatCode>[$-409]mmmm\ d\,\ yyyy;@</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>42699</c:v>
                 </c:pt>
@@ -1567,15 +1600,18 @@
                 <c:pt idx="3">
                   <c:v>42847</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>42855</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Progress!$C$48:$C$51</c:f>
+              <c:f>Progress!$C$48:$C$52</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1587,6 +1623,9 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>126</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>119</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1619,10 +1658,10 @@
           </c:spPr>
           <c:cat>
             <c:numRef>
-              <c:f>Progress!$A$48:$A$51</c:f>
+              <c:f>Progress!$A$48:$A$52</c:f>
               <c:numCache>
                 <c:formatCode>[$-409]mmmm\ d\,\ yyyy;@</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>42699</c:v>
                 </c:pt>
@@ -1635,15 +1674,18 @@
                 <c:pt idx="3">
                   <c:v>42847</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>42855</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Progress!$D$48:$D$51</c:f>
+              <c:f>Progress!$D$48:$D$52</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1656,15 +1698,18 @@
                 <c:pt idx="3">
                   <c:v>2</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="122362112"/>
-        <c:axId val="122368000"/>
+        <c:axId val="132835584"/>
+        <c:axId val="132841472"/>
       </c:areaChart>
       <c:dateAx>
-        <c:axId val="122362112"/>
+        <c:axId val="132835584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1697,7 +1742,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="122368000"/>
+        <c:crossAx val="132841472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -1708,7 +1753,7 @@
         <c:minorTimeUnit val="months"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="122368000"/>
+        <c:axId val="132841472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1750,7 +1795,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="122362112"/>
+        <c:crossAx val="132835584"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1799,7 +1844,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="1" l="0.75000000000001199" r="0.75000000000001199" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.7500000000000121" r="0.7500000000000121" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
   </c:printSettings>
 </c:chartSpace>
@@ -1849,7 +1894,7 @@
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>66</xdr:row>
+      <xdr:row>67</xdr:row>
       <xdr:rowOff>9524</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2259,8 +2304,8 @@
   </sheetPr>
   <dimension ref="A1:D412"/>
   <sheetViews>
-    <sheetView topLeftCell="A105" workbookViewId="0">
-      <selection activeCell="B153" sqref="B153"/>
+    <sheetView topLeftCell="A233" workbookViewId="0">
+      <selection activeCell="C268" sqref="C268"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5"/>
@@ -2433,7 +2478,7 @@
     </row>
     <row r="26" spans="2:4" s="6" customFormat="1">
       <c r="B26" s="22" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C26" s="7" t="s">
         <v>14</v>
@@ -2469,7 +2514,7 @@
     </row>
     <row r="30" spans="2:4" s="6" customFormat="1">
       <c r="B30" s="22" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C30" s="7" t="s">
         <v>14</v>
@@ -2478,7 +2523,7 @@
     </row>
     <row r="31" spans="2:4" s="6" customFormat="1">
       <c r="B31" s="22" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C31" s="7" t="s">
         <v>14</v>
@@ -2564,7 +2609,7 @@
     </row>
     <row r="43" spans="2:4" s="6" customFormat="1">
       <c r="B43" s="22" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C43" s="7" t="s">
         <v>14</v>
@@ -2573,7 +2618,7 @@
     </row>
     <row r="44" spans="2:4" s="6" customFormat="1">
       <c r="B44" s="22" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C44" s="7" t="s">
         <v>14</v>
@@ -2596,7 +2641,7 @@
     </row>
     <row r="47" spans="2:4" s="6" customFormat="1">
       <c r="B47" s="20" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C47" s="7" t="s">
         <v>14</v>
@@ -2677,7 +2722,7 @@
     </row>
     <row r="56" spans="2:4" s="6" customFormat="1">
       <c r="B56" s="22" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C56" s="7" t="s">
         <v>14</v>
@@ -2686,7 +2731,7 @@
     </row>
     <row r="57" spans="2:4" s="6" customFormat="1">
       <c r="B57" s="20" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C57" s="7" t="s">
         <v>14</v>
@@ -2695,7 +2740,7 @@
     </row>
     <row r="58" spans="2:4" s="6" customFormat="1">
       <c r="B58" s="20" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C58" s="7" t="s">
         <v>61</v>
@@ -2704,7 +2749,7 @@
     </row>
     <row r="59" spans="2:4" s="6" customFormat="1">
       <c r="B59" s="22" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C59" s="7" t="s">
         <v>14</v>
@@ -2727,7 +2772,7 @@
     </row>
     <row r="62" spans="2:4" s="6" customFormat="1">
       <c r="B62" s="20" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C62" s="7" t="s">
         <v>2</v>
@@ -2736,7 +2781,7 @@
     </row>
     <row r="63" spans="2:4" s="6" customFormat="1">
       <c r="B63" s="20" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C63" s="7" t="s">
         <v>14</v>
@@ -2745,7 +2790,7 @@
     </row>
     <row r="64" spans="2:4" s="6" customFormat="1">
       <c r="B64" s="20" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C64" s="7" t="s">
         <v>14</v>
@@ -3334,7 +3379,7 @@
     </row>
     <row r="153" spans="2:4" s="6" customFormat="1">
       <c r="B153" s="20" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C153" s="7" t="s">
         <v>14</v>
@@ -3774,41 +3819,53 @@
         <v>142</v>
       </c>
       <c r="C218" s="7" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D218" s="4"/>
     </row>
     <row r="219" spans="2:4" s="6" customFormat="1">
       <c r="B219" s="20" t="s">
-        <v>143</v>
+        <v>172</v>
       </c>
       <c r="C219" s="7" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D219" s="4"/>
     </row>
     <row r="220" spans="2:4" s="6" customFormat="1">
       <c r="B220" s="20" t="s">
-        <v>144</v>
+        <v>173</v>
       </c>
       <c r="C220" s="7" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D220" s="4"/>
     </row>
     <row r="221" spans="2:4" s="6" customFormat="1">
-      <c r="B221" s="20"/>
-      <c r="C221" s="7"/>
+      <c r="B221" s="22" t="s">
+        <v>174</v>
+      </c>
+      <c r="C221" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="D221" s="4"/>
     </row>
     <row r="222" spans="2:4" s="6" customFormat="1">
-      <c r="B222" s="20"/>
-      <c r="C222" s="7"/>
+      <c r="B222" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="C222" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="D222" s="4"/>
     </row>
     <row r="223" spans="2:4" s="6" customFormat="1">
-      <c r="B223" s="20"/>
-      <c r="C223" s="7"/>
+      <c r="B223" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="C223" s="7" t="s">
+        <v>2</v>
+      </c>
       <c r="D223" s="4"/>
     </row>
     <row r="224" spans="2:4" s="6" customFormat="1">
@@ -3883,7 +3940,7 @@
     </row>
     <row r="238" spans="2:4">
       <c r="B238" s="43" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C238" s="7"/>
     </row>
@@ -3926,16 +3983,16 @@
       <c r="B244" t="s">
         <v>92</v>
       </c>
-      <c r="C244" s="9" t="s">
-        <v>14</v>
+      <c r="C244" s="7" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="245" spans="2:3">
       <c r="B245" t="s">
         <v>93</v>
       </c>
-      <c r="C245" s="9" t="s">
-        <v>14</v>
+      <c r="C245" s="7" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="246" spans="2:3">
@@ -4028,7 +4085,7 @@
     </row>
     <row r="261" spans="2:3">
       <c r="B261" s="43" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C261" s="9"/>
     </row>
@@ -4085,10 +4142,10 @@
     </row>
     <row r="269" spans="2:3">
       <c r="B269" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C269" s="7" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
     <row r="270" spans="2:3">
@@ -4102,7 +4159,7 @@
     </row>
     <row r="273" spans="2:3">
       <c r="B273" s="43" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C273" s="9"/>
     </row>
@@ -4111,7 +4168,7 @@
     </row>
     <row r="275" spans="2:3">
       <c r="B275" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C275" s="9" t="s">
         <v>14</v>
@@ -4308,10 +4365,10 @@
     </row>
     <row r="319" spans="2:3">
       <c r="B319" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C319" s="7" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
     <row r="320" spans="2:3">
@@ -4407,7 +4464,7 @@
     </row>
     <row r="338" spans="2:4" s="6" customFormat="1">
       <c r="B338" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C338" s="7" t="s">
         <v>14</v>
@@ -4554,7 +4611,7 @@
     </row>
     <row r="359" spans="2:4" s="6" customFormat="1">
       <c r="B359" s="22" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C359" s="7" t="s">
         <v>14</v>
@@ -4598,7 +4655,7 @@
     </row>
     <row r="367" spans="2:4" s="6" customFormat="1">
       <c r="B367" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C367" s="7"/>
       <c r="D367" s="4"/>
@@ -4610,14 +4667,14 @@
     </row>
     <row r="369" spans="2:4" s="6" customFormat="1">
       <c r="B369" s="22" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C369" s="7"/>
       <c r="D369" s="4"/>
     </row>
     <row r="370" spans="2:4" s="6" customFormat="1">
       <c r="B370" s="20" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C370" s="7" t="s">
         <v>2</v>
@@ -4626,7 +4683,7 @@
     </row>
     <row r="371" spans="2:4" s="6" customFormat="1">
       <c r="B371" s="20" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C371" s="7" t="s">
         <v>2</v>
@@ -4635,7 +4692,7 @@
     </row>
     <row r="372" spans="2:4" s="6" customFormat="1">
       <c r="B372" s="20" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C372" s="7" t="s">
         <v>14</v>
@@ -4644,7 +4701,7 @@
     </row>
     <row r="373" spans="2:4" s="6" customFormat="1">
       <c r="B373" s="20" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C373" s="7" t="s">
         <v>2</v>
@@ -4665,7 +4722,7 @@
     </row>
     <row r="376" spans="2:4" s="6" customFormat="1">
       <c r="B376" s="20" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C376" s="7" t="s">
         <v>2</v>
@@ -4674,7 +4731,7 @@
     </row>
     <row r="377" spans="2:4" s="6" customFormat="1">
       <c r="B377" s="20" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C377" s="7" t="s">
         <v>2</v>
@@ -4834,7 +4891,7 @@
       </c>
       <c r="C407" s="6">
         <f>COUNTIF(C5:C406,"y")</f>
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="D407" s="2"/>
     </row>
@@ -4845,7 +4902,7 @@
       </c>
       <c r="C408" s="6">
         <f>COUNTIF(C5:C406,"n")</f>
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D408" s="2"/>
     </row>
@@ -4867,7 +4924,7 @@
       </c>
       <c r="C410">
         <f>SUM(C407:C409)</f>
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="D410" s="2"/>
     </row>
@@ -4879,7 +4936,7 @@
       </c>
       <c r="D411" s="41">
         <f>C407/(C408+C407 + C409)</f>
-        <v>0.2</v>
+        <v>0.25766871165644173</v>
       </c>
     </row>
     <row r="412" spans="1:4">
@@ -4912,12 +4969,12 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:IT865"/>
+  <dimension ref="A1:IT866"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="10020" topLeftCell="A46" activePane="bottomLeft"/>
       <selection activeCell="O27" sqref="O27"/>
-      <selection pane="bottomLeft" activeCell="D51" sqref="D51"/>
+      <selection pane="bottomLeft" activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5"/>
@@ -5252,13 +5309,28 @@
       <c r="H51" s="7"/>
     </row>
     <row r="52" spans="1:11">
-      <c r="A52" s="44"/>
-      <c r="B52" s="4"/>
-      <c r="C52" s="4"/>
-      <c r="D52" s="4"/>
-      <c r="E52" s="4"/>
-      <c r="F52" s="28"/>
-      <c r="G52" s="30"/>
+      <c r="A52" s="44">
+        <v>42855</v>
+      </c>
+      <c r="B52" s="4">
+        <v>42</v>
+      </c>
+      <c r="C52" s="4">
+        <v>119</v>
+      </c>
+      <c r="D52" s="4">
+        <v>2</v>
+      </c>
+      <c r="E52" s="4">
+        <v>0</v>
+      </c>
+      <c r="F52" s="28">
+        <v>0</v>
+      </c>
+      <c r="G52" s="30">
+        <f t="shared" ref="G52" si="3">B52/SUM(B52:E52)</f>
+        <v>0.25766871165644173</v>
+      </c>
       <c r="H52" s="7"/>
     </row>
     <row r="53" spans="1:11">
@@ -5267,84 +5339,84 @@
       <c r="C53" s="4"/>
       <c r="D53" s="4"/>
       <c r="E53" s="4"/>
-      <c r="F53" s="31"/>
+      <c r="F53" s="28"/>
       <c r="G53" s="30"/>
       <c r="H53" s="7"/>
     </row>
     <row r="54" spans="1:11">
-      <c r="A54" s="14" t="s">
+      <c r="A54" s="44"/>
+      <c r="B54" s="4"/>
+      <c r="C54" s="4"/>
+      <c r="D54" s="4"/>
+      <c r="E54" s="4"/>
+      <c r="F54" s="31"/>
+      <c r="G54" s="30"/>
+      <c r="H54" s="7"/>
+    </row>
+    <row r="55" spans="1:11">
+      <c r="A55" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="B54" s="14" t="s">
+      <c r="B55" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C54" s="14" t="s">
+      <c r="C55" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D54" s="14" t="s">
+      <c r="D55" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E54" s="14" t="s">
+      <c r="E55" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="F54" s="14" t="s">
+      <c r="F55" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="G54" s="38">
-        <f>MIN(G51)</f>
-        <v>0.2</v>
-      </c>
-      <c r="H54" s="7"/>
-    </row>
-    <row r="55" spans="1:11">
-      <c r="A55" s="39">
-        <f>SUM(B55:D55)</f>
-        <v>160</v>
-      </c>
-      <c r="B55" s="15">
+      <c r="G55" s="38">
+        <f>MIN(G52)</f>
+        <v>0.25766871165644173</v>
+      </c>
+      <c r="H55" s="7"/>
+    </row>
+    <row r="56" spans="1:11">
+      <c r="A56" s="39">
+        <f>SUM(B56:D56)</f>
+        <v>163</v>
+      </c>
+      <c r="B56" s="15">
         <f>Features!C407</f>
-        <v>32</v>
-      </c>
-      <c r="C55" s="16">
+        <v>42</v>
+      </c>
+      <c r="C56" s="16">
         <f>Features!C408</f>
-        <v>126</v>
-      </c>
-      <c r="D55" s="17">
+        <v>119</v>
+      </c>
+      <c r="D56" s="17">
         <f>Features!C409</f>
         <v>2</v>
       </c>
-      <c r="E55" s="18">
-        <f>MIN(E51)</f>
+      <c r="E56" s="18">
+        <f>MIN(E52)</f>
         <v>0</v>
       </c>
-      <c r="F55" s="7"/>
-      <c r="G55" s="30"/>
-      <c r="H55" s="7"/>
-    </row>
-    <row r="56" spans="1:11">
-      <c r="A56" s="4"/>
-      <c r="B56" s="19"/>
-      <c r="C56" s="4"/>
-      <c r="D56" s="7"/>
-      <c r="E56" s="7"/>
       <c r="F56" s="7"/>
       <c r="G56" s="30"/>
       <c r="H56" s="7"/>
-      <c r="J56" s="36"/>
     </row>
     <row r="57" spans="1:11">
       <c r="A57" s="4"/>
-      <c r="B57" s="4"/>
+      <c r="B57" s="19"/>
       <c r="C57" s="4"/>
       <c r="D57" s="7"/>
       <c r="E57" s="7"/>
       <c r="F57" s="7"/>
       <c r="G57" s="30"/>
       <c r="H57" s="7"/>
+      <c r="J57" s="36"/>
     </row>
     <row r="58" spans="1:11">
       <c r="A58" s="4"/>
-      <c r="B58" s="19"/>
+      <c r="B58" s="4"/>
       <c r="C58" s="4"/>
       <c r="D58" s="7"/>
       <c r="E58" s="7"/>
@@ -5353,13 +5425,8 @@
       <c r="H58" s="7"/>
     </row>
     <row r="59" spans="1:11">
-      <c r="A59" s="48" t="s">
-        <v>154</v>
-      </c>
-      <c r="B59" s="47">
-        <f>A48+A55/B55*(A51-A48)</f>
-        <v>43439</v>
-      </c>
+      <c r="A59" s="4"/>
+      <c r="B59" s="19"/>
       <c r="C59" s="4"/>
       <c r="D59" s="7"/>
       <c r="E59" s="7"/>
@@ -5368,8 +5435,13 @@
       <c r="H59" s="7"/>
     </row>
     <row r="60" spans="1:11">
-      <c r="A60" s="4"/>
-      <c r="B60" s="4"/>
+      <c r="A60" s="48" t="s">
+        <v>152</v>
+      </c>
+      <c r="B60" s="47">
+        <f>A48+A56/B56*(A52-A48)</f>
+        <v>43304.428571428572</v>
+      </c>
       <c r="C60" s="4"/>
       <c r="D60" s="7"/>
       <c r="E60" s="7"/>
@@ -5379,7 +5451,7 @@
     </row>
     <row r="61" spans="1:11">
       <c r="A61" s="4"/>
-      <c r="B61" s="19"/>
+      <c r="B61" s="4"/>
       <c r="C61" s="4"/>
       <c r="D61" s="7"/>
       <c r="E61" s="7"/>
@@ -5399,7 +5471,7 @@
     </row>
     <row r="63" spans="1:11">
       <c r="A63" s="4"/>
-      <c r="B63" s="4"/>
+      <c r="B63" s="19"/>
       <c r="C63" s="4"/>
       <c r="D63" s="7"/>
       <c r="E63" s="7"/>
@@ -5419,7 +5491,7 @@
     </row>
     <row r="65" spans="1:8">
       <c r="A65" s="4"/>
-      <c r="B65" s="7"/>
+      <c r="B65" s="4"/>
       <c r="C65" s="4"/>
       <c r="D65" s="7"/>
       <c r="E65" s="7"/>
@@ -5429,7 +5501,7 @@
     </row>
     <row r="66" spans="1:8">
       <c r="A66" s="4"/>
-      <c r="B66" s="20"/>
+      <c r="B66" s="7"/>
       <c r="C66" s="4"/>
       <c r="D66" s="7"/>
       <c r="E66" s="7"/>
@@ -5448,7 +5520,7 @@
       <c r="H67" s="7"/>
     </row>
     <row r="68" spans="1:8">
-      <c r="A68" s="7"/>
+      <c r="A68" s="4"/>
       <c r="B68" s="20"/>
       <c r="C68" s="4"/>
       <c r="D68" s="7"/>
@@ -5459,7 +5531,7 @@
     </row>
     <row r="69" spans="1:8">
       <c r="A69" s="7"/>
-      <c r="B69" s="7"/>
+      <c r="B69" s="20"/>
       <c r="C69" s="4"/>
       <c r="D69" s="7"/>
       <c r="E69" s="7"/>
@@ -5590,7 +5662,7 @@
     <row r="82" spans="1:8">
       <c r="A82" s="7"/>
       <c r="B82" s="7"/>
-      <c r="C82" s="7"/>
+      <c r="C82" s="4"/>
       <c r="D82" s="7"/>
       <c r="E82" s="7"/>
       <c r="F82" s="7"/>
@@ -5599,7 +5671,7 @@
     </row>
     <row r="83" spans="1:8">
       <c r="A83" s="7"/>
-      <c r="B83" s="6"/>
+      <c r="B83" s="7"/>
       <c r="C83" s="7"/>
       <c r="D83" s="7"/>
       <c r="E83" s="7"/>
@@ -5607,15 +5679,15 @@
       <c r="G83" s="30"/>
       <c r="H83" s="7"/>
     </row>
-    <row r="84" spans="1:8" s="2" customFormat="1">
-      <c r="A84" s="4"/>
-      <c r="B84" s="4"/>
-      <c r="C84" s="4"/>
-      <c r="D84" s="4"/>
-      <c r="E84" s="4"/>
-      <c r="F84" s="4"/>
-      <c r="G84" s="34"/>
-      <c r="H84" s="4"/>
+    <row r="84" spans="1:8">
+      <c r="A84" s="7"/>
+      <c r="B84" s="6"/>
+      <c r="C84" s="7"/>
+      <c r="D84" s="7"/>
+      <c r="E84" s="7"/>
+      <c r="F84" s="7"/>
+      <c r="G84" s="30"/>
+      <c r="H84" s="7"/>
     </row>
     <row r="85" spans="1:8" s="2" customFormat="1">
       <c r="A85" s="4"/>
@@ -5789,7 +5861,7 @@
     </row>
     <row r="102" spans="1:8" s="2" customFormat="1">
       <c r="A102" s="4"/>
-      <c r="B102" s="6"/>
+      <c r="B102" s="4"/>
       <c r="C102" s="4"/>
       <c r="D102" s="4"/>
       <c r="E102" s="4"/>
@@ -5799,7 +5871,7 @@
     </row>
     <row r="103" spans="1:8" s="2" customFormat="1">
       <c r="A103" s="4"/>
-      <c r="B103" s="4"/>
+      <c r="B103" s="6"/>
       <c r="C103" s="4"/>
       <c r="D103" s="4"/>
       <c r="E103" s="4"/>
@@ -5829,7 +5901,7 @@
     </row>
     <row r="106" spans="1:8" s="2" customFormat="1">
       <c r="A106" s="4"/>
-      <c r="B106" s="19"/>
+      <c r="B106" s="4"/>
       <c r="C106" s="4"/>
       <c r="D106" s="4"/>
       <c r="E106" s="4"/>
@@ -5869,7 +5941,7 @@
     </row>
     <row r="110" spans="1:8" s="2" customFormat="1">
       <c r="A110" s="4"/>
-      <c r="B110" s="21"/>
+      <c r="B110" s="19"/>
       <c r="C110" s="4"/>
       <c r="D110" s="4"/>
       <c r="E110" s="4"/>
@@ -5879,7 +5951,7 @@
     </row>
     <row r="111" spans="1:8" s="2" customFormat="1">
       <c r="A111" s="4"/>
-      <c r="B111" s="4"/>
+      <c r="B111" s="21"/>
       <c r="C111" s="4"/>
       <c r="D111" s="4"/>
       <c r="E111" s="4"/>
@@ -5889,7 +5961,7 @@
     </row>
     <row r="112" spans="1:8" s="2" customFormat="1">
       <c r="A112" s="4"/>
-      <c r="B112" s="6"/>
+      <c r="B112" s="4"/>
       <c r="C112" s="4"/>
       <c r="D112" s="4"/>
       <c r="E112" s="4"/>
@@ -5899,7 +5971,7 @@
     </row>
     <row r="113" spans="1:8" s="2" customFormat="1">
       <c r="A113" s="4"/>
-      <c r="B113" s="4"/>
+      <c r="B113" s="6"/>
       <c r="C113" s="4"/>
       <c r="D113" s="4"/>
       <c r="E113" s="4"/>
@@ -5909,7 +5981,7 @@
     </row>
     <row r="114" spans="1:8" s="2" customFormat="1">
       <c r="A114" s="4"/>
-      <c r="B114" s="19"/>
+      <c r="B114" s="4"/>
       <c r="C114" s="4"/>
       <c r="D114" s="4"/>
       <c r="E114" s="4"/>
@@ -5929,7 +6001,7 @@
     </row>
     <row r="116" spans="1:8" s="2" customFormat="1">
       <c r="A116" s="4"/>
-      <c r="B116" s="4"/>
+      <c r="B116" s="19"/>
       <c r="C116" s="4"/>
       <c r="D116" s="4"/>
       <c r="E116" s="4"/>
@@ -5989,7 +6061,7 @@
     </row>
     <row r="122" spans="1:8" s="2" customFormat="1">
       <c r="A122" s="4"/>
-      <c r="B122" s="19"/>
+      <c r="B122" s="4"/>
       <c r="C122" s="4"/>
       <c r="D122" s="4"/>
       <c r="E122" s="4"/>
@@ -6089,7 +6161,7 @@
     </row>
     <row r="132" spans="1:254" s="2" customFormat="1">
       <c r="A132" s="4"/>
-      <c r="B132" s="4"/>
+      <c r="B132" s="19"/>
       <c r="C132" s="4"/>
       <c r="D132" s="4"/>
       <c r="E132" s="4"/>
@@ -6139,7 +6211,7 @@
     </row>
     <row r="137" spans="1:254" s="2" customFormat="1">
       <c r="A137" s="4"/>
-      <c r="B137" s="19"/>
+      <c r="B137" s="4"/>
       <c r="C137" s="4"/>
       <c r="D137" s="4"/>
       <c r="E137" s="4"/>
@@ -6159,7 +6231,7 @@
     </row>
     <row r="139" spans="1:254" s="2" customFormat="1">
       <c r="A139" s="4"/>
-      <c r="B139" s="4"/>
+      <c r="B139" s="19"/>
       <c r="C139" s="4"/>
       <c r="D139" s="4"/>
       <c r="E139" s="4"/>
@@ -6198,284 +6270,284 @@
       <c r="H142" s="4"/>
     </row>
     <row r="143" spans="1:254" s="2" customFormat="1">
-      <c r="A143" s="21"/>
-      <c r="B143" s="21"/>
-      <c r="C143" s="21"/>
-      <c r="D143" s="21"/>
-      <c r="E143" s="21"/>
-      <c r="F143" s="21"/>
-      <c r="G143" s="35"/>
-      <c r="H143" s="21"/>
-      <c r="I143" s="5"/>
-      <c r="J143" s="5"/>
-      <c r="K143" s="5"/>
-      <c r="L143" s="5"/>
-      <c r="M143" s="5"/>
-      <c r="N143" s="5"/>
-      <c r="O143" s="5"/>
-      <c r="P143" s="5"/>
-      <c r="Q143" s="5"/>
-      <c r="R143" s="5"/>
-      <c r="S143" s="5"/>
-      <c r="T143" s="5"/>
-      <c r="U143" s="5"/>
-      <c r="V143" s="5"/>
-      <c r="W143" s="5"/>
-      <c r="X143" s="5"/>
-      <c r="Y143" s="5"/>
-      <c r="Z143" s="5"/>
-      <c r="AA143" s="5"/>
-      <c r="AB143" s="5"/>
-      <c r="AC143" s="5"/>
-      <c r="AD143" s="5"/>
-      <c r="AE143" s="5"/>
-      <c r="AF143" s="5"/>
-      <c r="AG143" s="5"/>
-      <c r="AH143" s="5"/>
-      <c r="AI143" s="5"/>
-      <c r="AJ143" s="5"/>
-      <c r="AK143" s="5"/>
-      <c r="AL143" s="5"/>
-      <c r="AM143" s="5"/>
-      <c r="AN143" s="5"/>
-      <c r="AO143" s="5"/>
-      <c r="AP143" s="5"/>
-      <c r="AQ143" s="5"/>
-      <c r="AR143" s="5"/>
-      <c r="AS143" s="5"/>
-      <c r="AT143" s="5"/>
-      <c r="AU143" s="5"/>
-      <c r="AV143" s="5"/>
-      <c r="AW143" s="5"/>
-      <c r="AX143" s="5"/>
-      <c r="AY143" s="5"/>
-      <c r="AZ143" s="5"/>
-      <c r="BA143" s="5"/>
-      <c r="BB143" s="5"/>
-      <c r="BC143" s="5"/>
-      <c r="BD143" s="5"/>
-      <c r="BE143" s="5"/>
-      <c r="BF143" s="5"/>
-      <c r="BG143" s="5"/>
-      <c r="BH143" s="5"/>
-      <c r="BI143" s="5"/>
-      <c r="BJ143" s="5"/>
-      <c r="BK143" s="5"/>
-      <c r="BL143" s="5"/>
-      <c r="BM143" s="5"/>
-      <c r="BN143" s="5"/>
-      <c r="BO143" s="5"/>
-      <c r="BP143" s="5"/>
-      <c r="BQ143" s="5"/>
-      <c r="BR143" s="5"/>
-      <c r="BS143" s="5"/>
-      <c r="BT143" s="5"/>
-      <c r="BU143" s="5"/>
-      <c r="BV143" s="5"/>
-      <c r="BW143" s="5"/>
-      <c r="BX143" s="5"/>
-      <c r="BY143" s="5"/>
-      <c r="BZ143" s="5"/>
-      <c r="CA143" s="5"/>
-      <c r="CB143" s="5"/>
-      <c r="CC143" s="5"/>
-      <c r="CD143" s="5"/>
-      <c r="CE143" s="5"/>
-      <c r="CF143" s="5"/>
-      <c r="CG143" s="5"/>
-      <c r="CH143" s="5"/>
-      <c r="CI143" s="5"/>
-      <c r="CJ143" s="5"/>
-      <c r="CK143" s="5"/>
-      <c r="CL143" s="5"/>
-      <c r="CM143" s="5"/>
-      <c r="CN143" s="5"/>
-      <c r="CO143" s="5"/>
-      <c r="CP143" s="5"/>
-      <c r="CQ143" s="5"/>
-      <c r="CR143" s="5"/>
-      <c r="CS143" s="5"/>
-      <c r="CT143" s="5"/>
-      <c r="CU143" s="5"/>
-      <c r="CV143" s="5"/>
-      <c r="CW143" s="5"/>
-      <c r="CX143" s="5"/>
-      <c r="CY143" s="5"/>
-      <c r="CZ143" s="5"/>
-      <c r="DA143" s="5"/>
-      <c r="DB143" s="5"/>
-      <c r="DC143" s="5"/>
-      <c r="DD143" s="5"/>
-      <c r="DE143" s="5"/>
-      <c r="DF143" s="5"/>
-      <c r="DG143" s="5"/>
-      <c r="DH143" s="5"/>
-      <c r="DI143" s="5"/>
-      <c r="DJ143" s="5"/>
-      <c r="DK143" s="5"/>
-      <c r="DL143" s="5"/>
-      <c r="DM143" s="5"/>
-      <c r="DN143" s="5"/>
-      <c r="DO143" s="5"/>
-      <c r="DP143" s="5"/>
-      <c r="DQ143" s="5"/>
-      <c r="DR143" s="5"/>
-      <c r="DS143" s="5"/>
-      <c r="DT143" s="5"/>
-      <c r="DU143" s="5"/>
-      <c r="DV143" s="5"/>
-      <c r="DW143" s="5"/>
-      <c r="DX143" s="5"/>
-      <c r="DY143" s="5"/>
-      <c r="DZ143" s="5"/>
-      <c r="EA143" s="5"/>
-      <c r="EB143" s="5"/>
-      <c r="EC143" s="5"/>
-      <c r="ED143" s="5"/>
-      <c r="EE143" s="5"/>
-      <c r="EF143" s="5"/>
-      <c r="EG143" s="5"/>
-      <c r="EH143" s="5"/>
-      <c r="EI143" s="5"/>
-      <c r="EJ143" s="5"/>
-      <c r="EK143" s="5"/>
-      <c r="EL143" s="5"/>
-      <c r="EM143" s="5"/>
-      <c r="EN143" s="5"/>
-      <c r="EO143" s="5"/>
-      <c r="EP143" s="5"/>
-      <c r="EQ143" s="5"/>
-      <c r="ER143" s="5"/>
-      <c r="ES143" s="5"/>
-      <c r="ET143" s="5"/>
-      <c r="EU143" s="5"/>
-      <c r="EV143" s="5"/>
-      <c r="EW143" s="5"/>
-      <c r="EX143" s="5"/>
-      <c r="EY143" s="5"/>
-      <c r="EZ143" s="5"/>
-      <c r="FA143" s="5"/>
-      <c r="FB143" s="5"/>
-      <c r="FC143" s="5"/>
-      <c r="FD143" s="5"/>
-      <c r="FE143" s="5"/>
-      <c r="FF143" s="5"/>
-      <c r="FG143" s="5"/>
-      <c r="FH143" s="5"/>
-      <c r="FI143" s="5"/>
-      <c r="FJ143" s="5"/>
-      <c r="FK143" s="5"/>
-      <c r="FL143" s="5"/>
-      <c r="FM143" s="5"/>
-      <c r="FN143" s="5"/>
-      <c r="FO143" s="5"/>
-      <c r="FP143" s="5"/>
-      <c r="FQ143" s="5"/>
-      <c r="FR143" s="5"/>
-      <c r="FS143" s="5"/>
-      <c r="FT143" s="5"/>
-      <c r="FU143" s="5"/>
-      <c r="FV143" s="5"/>
-      <c r="FW143" s="5"/>
-      <c r="FX143" s="5"/>
-      <c r="FY143" s="5"/>
-      <c r="FZ143" s="5"/>
-      <c r="GA143" s="5"/>
-      <c r="GB143" s="5"/>
-      <c r="GC143" s="5"/>
-      <c r="GD143" s="5"/>
-      <c r="GE143" s="5"/>
-      <c r="GF143" s="5"/>
-      <c r="GG143" s="5"/>
-      <c r="GH143" s="5"/>
-      <c r="GI143" s="5"/>
-      <c r="GJ143" s="5"/>
-      <c r="GK143" s="5"/>
-      <c r="GL143" s="5"/>
-      <c r="GM143" s="5"/>
-      <c r="GN143" s="5"/>
-      <c r="GO143" s="5"/>
-      <c r="GP143" s="5"/>
-      <c r="GQ143" s="5"/>
-      <c r="GR143" s="5"/>
-      <c r="GS143" s="5"/>
-      <c r="GT143" s="5"/>
-      <c r="GU143" s="5"/>
-      <c r="GV143" s="5"/>
-      <c r="GW143" s="5"/>
-      <c r="GX143" s="5"/>
-      <c r="GY143" s="5"/>
-      <c r="GZ143" s="5"/>
-      <c r="HA143" s="5"/>
-      <c r="HB143" s="5"/>
-      <c r="HC143" s="5"/>
-      <c r="HD143" s="5"/>
-      <c r="HE143" s="5"/>
-      <c r="HF143" s="5"/>
-      <c r="HG143" s="5"/>
-      <c r="HH143" s="5"/>
-      <c r="HI143" s="5"/>
-      <c r="HJ143" s="5"/>
-      <c r="HK143" s="5"/>
-      <c r="HL143" s="5"/>
-      <c r="HM143" s="5"/>
-      <c r="HN143" s="5"/>
-      <c r="HO143" s="5"/>
-      <c r="HP143" s="5"/>
-      <c r="HQ143" s="5"/>
-      <c r="HR143" s="5"/>
-      <c r="HS143" s="5"/>
-      <c r="HT143" s="5"/>
-      <c r="HU143" s="5"/>
-      <c r="HV143" s="5"/>
-      <c r="HW143" s="5"/>
-      <c r="HX143" s="5"/>
-      <c r="HY143" s="5"/>
-      <c r="HZ143" s="5"/>
-      <c r="IA143" s="5"/>
-      <c r="IB143" s="5"/>
-      <c r="IC143" s="5"/>
-      <c r="ID143" s="5"/>
-      <c r="IE143" s="5"/>
-      <c r="IF143" s="5"/>
-      <c r="IG143" s="5"/>
-      <c r="IH143" s="5"/>
-      <c r="II143" s="5"/>
-      <c r="IJ143" s="5"/>
-      <c r="IK143" s="5"/>
-      <c r="IL143" s="5"/>
-      <c r="IM143" s="5"/>
-      <c r="IN143" s="5"/>
-      <c r="IO143" s="5"/>
-      <c r="IP143" s="5"/>
-      <c r="IQ143" s="5"/>
-      <c r="IR143" s="5"/>
-      <c r="IS143" s="5"/>
-      <c r="IT143" s="5"/>
+      <c r="A143" s="4"/>
+      <c r="B143" s="4"/>
+      <c r="C143" s="4"/>
+      <c r="D143" s="4"/>
+      <c r="E143" s="4"/>
+      <c r="F143" s="4"/>
+      <c r="G143" s="34"/>
+      <c r="H143" s="4"/>
     </row>
     <row r="144" spans="1:254" s="2" customFormat="1">
-      <c r="A144" s="4"/>
-      <c r="B144" s="4"/>
-      <c r="C144" s="4"/>
-      <c r="D144" s="4"/>
-      <c r="E144" s="4"/>
-      <c r="F144" s="4"/>
-      <c r="G144" s="34"/>
-      <c r="H144" s="4"/>
-    </row>
-    <row r="145" spans="1:8">
-      <c r="A145" s="7"/>
-      <c r="B145" s="6"/>
-      <c r="C145" s="7"/>
-      <c r="D145" s="7"/>
-      <c r="E145" s="7"/>
-      <c r="F145" s="7"/>
-      <c r="G145" s="30"/>
-      <c r="H145" s="7"/>
+      <c r="A144" s="21"/>
+      <c r="B144" s="21"/>
+      <c r="C144" s="21"/>
+      <c r="D144" s="21"/>
+      <c r="E144" s="21"/>
+      <c r="F144" s="21"/>
+      <c r="G144" s="35"/>
+      <c r="H144" s="21"/>
+      <c r="I144" s="5"/>
+      <c r="J144" s="5"/>
+      <c r="K144" s="5"/>
+      <c r="L144" s="5"/>
+      <c r="M144" s="5"/>
+      <c r="N144" s="5"/>
+      <c r="O144" s="5"/>
+      <c r="P144" s="5"/>
+      <c r="Q144" s="5"/>
+      <c r="R144" s="5"/>
+      <c r="S144" s="5"/>
+      <c r="T144" s="5"/>
+      <c r="U144" s="5"/>
+      <c r="V144" s="5"/>
+      <c r="W144" s="5"/>
+      <c r="X144" s="5"/>
+      <c r="Y144" s="5"/>
+      <c r="Z144" s="5"/>
+      <c r="AA144" s="5"/>
+      <c r="AB144" s="5"/>
+      <c r="AC144" s="5"/>
+      <c r="AD144" s="5"/>
+      <c r="AE144" s="5"/>
+      <c r="AF144" s="5"/>
+      <c r="AG144" s="5"/>
+      <c r="AH144" s="5"/>
+      <c r="AI144" s="5"/>
+      <c r="AJ144" s="5"/>
+      <c r="AK144" s="5"/>
+      <c r="AL144" s="5"/>
+      <c r="AM144" s="5"/>
+      <c r="AN144" s="5"/>
+      <c r="AO144" s="5"/>
+      <c r="AP144" s="5"/>
+      <c r="AQ144" s="5"/>
+      <c r="AR144" s="5"/>
+      <c r="AS144" s="5"/>
+      <c r="AT144" s="5"/>
+      <c r="AU144" s="5"/>
+      <c r="AV144" s="5"/>
+      <c r="AW144" s="5"/>
+      <c r="AX144" s="5"/>
+      <c r="AY144" s="5"/>
+      <c r="AZ144" s="5"/>
+      <c r="BA144" s="5"/>
+      <c r="BB144" s="5"/>
+      <c r="BC144" s="5"/>
+      <c r="BD144" s="5"/>
+      <c r="BE144" s="5"/>
+      <c r="BF144" s="5"/>
+      <c r="BG144" s="5"/>
+      <c r="BH144" s="5"/>
+      <c r="BI144" s="5"/>
+      <c r="BJ144" s="5"/>
+      <c r="BK144" s="5"/>
+      <c r="BL144" s="5"/>
+      <c r="BM144" s="5"/>
+      <c r="BN144" s="5"/>
+      <c r="BO144" s="5"/>
+      <c r="BP144" s="5"/>
+      <c r="BQ144" s="5"/>
+      <c r="BR144" s="5"/>
+      <c r="BS144" s="5"/>
+      <c r="BT144" s="5"/>
+      <c r="BU144" s="5"/>
+      <c r="BV144" s="5"/>
+      <c r="BW144" s="5"/>
+      <c r="BX144" s="5"/>
+      <c r="BY144" s="5"/>
+      <c r="BZ144" s="5"/>
+      <c r="CA144" s="5"/>
+      <c r="CB144" s="5"/>
+      <c r="CC144" s="5"/>
+      <c r="CD144" s="5"/>
+      <c r="CE144" s="5"/>
+      <c r="CF144" s="5"/>
+      <c r="CG144" s="5"/>
+      <c r="CH144" s="5"/>
+      <c r="CI144" s="5"/>
+      <c r="CJ144" s="5"/>
+      <c r="CK144" s="5"/>
+      <c r="CL144" s="5"/>
+      <c r="CM144" s="5"/>
+      <c r="CN144" s="5"/>
+      <c r="CO144" s="5"/>
+      <c r="CP144" s="5"/>
+      <c r="CQ144" s="5"/>
+      <c r="CR144" s="5"/>
+      <c r="CS144" s="5"/>
+      <c r="CT144" s="5"/>
+      <c r="CU144" s="5"/>
+      <c r="CV144" s="5"/>
+      <c r="CW144" s="5"/>
+      <c r="CX144" s="5"/>
+      <c r="CY144" s="5"/>
+      <c r="CZ144" s="5"/>
+      <c r="DA144" s="5"/>
+      <c r="DB144" s="5"/>
+      <c r="DC144" s="5"/>
+      <c r="DD144" s="5"/>
+      <c r="DE144" s="5"/>
+      <c r="DF144" s="5"/>
+      <c r="DG144" s="5"/>
+      <c r="DH144" s="5"/>
+      <c r="DI144" s="5"/>
+      <c r="DJ144" s="5"/>
+      <c r="DK144" s="5"/>
+      <c r="DL144" s="5"/>
+      <c r="DM144" s="5"/>
+      <c r="DN144" s="5"/>
+      <c r="DO144" s="5"/>
+      <c r="DP144" s="5"/>
+      <c r="DQ144" s="5"/>
+      <c r="DR144" s="5"/>
+      <c r="DS144" s="5"/>
+      <c r="DT144" s="5"/>
+      <c r="DU144" s="5"/>
+      <c r="DV144" s="5"/>
+      <c r="DW144" s="5"/>
+      <c r="DX144" s="5"/>
+      <c r="DY144" s="5"/>
+      <c r="DZ144" s="5"/>
+      <c r="EA144" s="5"/>
+      <c r="EB144" s="5"/>
+      <c r="EC144" s="5"/>
+      <c r="ED144" s="5"/>
+      <c r="EE144" s="5"/>
+      <c r="EF144" s="5"/>
+      <c r="EG144" s="5"/>
+      <c r="EH144" s="5"/>
+      <c r="EI144" s="5"/>
+      <c r="EJ144" s="5"/>
+      <c r="EK144" s="5"/>
+      <c r="EL144" s="5"/>
+      <c r="EM144" s="5"/>
+      <c r="EN144" s="5"/>
+      <c r="EO144" s="5"/>
+      <c r="EP144" s="5"/>
+      <c r="EQ144" s="5"/>
+      <c r="ER144" s="5"/>
+      <c r="ES144" s="5"/>
+      <c r="ET144" s="5"/>
+      <c r="EU144" s="5"/>
+      <c r="EV144" s="5"/>
+      <c r="EW144" s="5"/>
+      <c r="EX144" s="5"/>
+      <c r="EY144" s="5"/>
+      <c r="EZ144" s="5"/>
+      <c r="FA144" s="5"/>
+      <c r="FB144" s="5"/>
+      <c r="FC144" s="5"/>
+      <c r="FD144" s="5"/>
+      <c r="FE144" s="5"/>
+      <c r="FF144" s="5"/>
+      <c r="FG144" s="5"/>
+      <c r="FH144" s="5"/>
+      <c r="FI144" s="5"/>
+      <c r="FJ144" s="5"/>
+      <c r="FK144" s="5"/>
+      <c r="FL144" s="5"/>
+      <c r="FM144" s="5"/>
+      <c r="FN144" s="5"/>
+      <c r="FO144" s="5"/>
+      <c r="FP144" s="5"/>
+      <c r="FQ144" s="5"/>
+      <c r="FR144" s="5"/>
+      <c r="FS144" s="5"/>
+      <c r="FT144" s="5"/>
+      <c r="FU144" s="5"/>
+      <c r="FV144" s="5"/>
+      <c r="FW144" s="5"/>
+      <c r="FX144" s="5"/>
+      <c r="FY144" s="5"/>
+      <c r="FZ144" s="5"/>
+      <c r="GA144" s="5"/>
+      <c r="GB144" s="5"/>
+      <c r="GC144" s="5"/>
+      <c r="GD144" s="5"/>
+      <c r="GE144" s="5"/>
+      <c r="GF144" s="5"/>
+      <c r="GG144" s="5"/>
+      <c r="GH144" s="5"/>
+      <c r="GI144" s="5"/>
+      <c r="GJ144" s="5"/>
+      <c r="GK144" s="5"/>
+      <c r="GL144" s="5"/>
+      <c r="GM144" s="5"/>
+      <c r="GN144" s="5"/>
+      <c r="GO144" s="5"/>
+      <c r="GP144" s="5"/>
+      <c r="GQ144" s="5"/>
+      <c r="GR144" s="5"/>
+      <c r="GS144" s="5"/>
+      <c r="GT144" s="5"/>
+      <c r="GU144" s="5"/>
+      <c r="GV144" s="5"/>
+      <c r="GW144" s="5"/>
+      <c r="GX144" s="5"/>
+      <c r="GY144" s="5"/>
+      <c r="GZ144" s="5"/>
+      <c r="HA144" s="5"/>
+      <c r="HB144" s="5"/>
+      <c r="HC144" s="5"/>
+      <c r="HD144" s="5"/>
+      <c r="HE144" s="5"/>
+      <c r="HF144" s="5"/>
+      <c r="HG144" s="5"/>
+      <c r="HH144" s="5"/>
+      <c r="HI144" s="5"/>
+      <c r="HJ144" s="5"/>
+      <c r="HK144" s="5"/>
+      <c r="HL144" s="5"/>
+      <c r="HM144" s="5"/>
+      <c r="HN144" s="5"/>
+      <c r="HO144" s="5"/>
+      <c r="HP144" s="5"/>
+      <c r="HQ144" s="5"/>
+      <c r="HR144" s="5"/>
+      <c r="HS144" s="5"/>
+      <c r="HT144" s="5"/>
+      <c r="HU144" s="5"/>
+      <c r="HV144" s="5"/>
+      <c r="HW144" s="5"/>
+      <c r="HX144" s="5"/>
+      <c r="HY144" s="5"/>
+      <c r="HZ144" s="5"/>
+      <c r="IA144" s="5"/>
+      <c r="IB144" s="5"/>
+      <c r="IC144" s="5"/>
+      <c r="ID144" s="5"/>
+      <c r="IE144" s="5"/>
+      <c r="IF144" s="5"/>
+      <c r="IG144" s="5"/>
+      <c r="IH144" s="5"/>
+      <c r="II144" s="5"/>
+      <c r="IJ144" s="5"/>
+      <c r="IK144" s="5"/>
+      <c r="IL144" s="5"/>
+      <c r="IM144" s="5"/>
+      <c r="IN144" s="5"/>
+      <c r="IO144" s="5"/>
+      <c r="IP144" s="5"/>
+      <c r="IQ144" s="5"/>
+      <c r="IR144" s="5"/>
+      <c r="IS144" s="5"/>
+      <c r="IT144" s="5"/>
+    </row>
+    <row r="145" spans="1:8" s="2" customFormat="1">
+      <c r="A145" s="4"/>
+      <c r="B145" s="4"/>
+      <c r="C145" s="4"/>
+      <c r="D145" s="4"/>
+      <c r="E145" s="4"/>
+      <c r="F145" s="4"/>
+      <c r="G145" s="34"/>
+      <c r="H145" s="4"/>
     </row>
     <row r="146" spans="1:8">
       <c r="A146" s="7"/>
-      <c r="B146" s="7"/>
+      <c r="B146" s="6"/>
       <c r="C146" s="7"/>
       <c r="D146" s="7"/>
       <c r="E146" s="7"/>
@@ -6485,7 +6557,7 @@
     </row>
     <row r="147" spans="1:8">
       <c r="A147" s="7"/>
-      <c r="B147" s="20"/>
+      <c r="B147" s="7"/>
       <c r="C147" s="7"/>
       <c r="D147" s="7"/>
       <c r="E147" s="7"/>
@@ -6495,7 +6567,7 @@
     </row>
     <row r="148" spans="1:8">
       <c r="A148" s="7"/>
-      <c r="B148" s="7"/>
+      <c r="B148" s="20"/>
       <c r="C148" s="7"/>
       <c r="D148" s="7"/>
       <c r="E148" s="7"/>
@@ -6506,7 +6578,7 @@
     <row r="149" spans="1:8">
       <c r="A149" s="7"/>
       <c r="B149" s="7"/>
-      <c r="C149" s="4"/>
+      <c r="C149" s="7"/>
       <c r="D149" s="7"/>
       <c r="E149" s="7"/>
       <c r="F149" s="7"/>
@@ -6546,7 +6618,7 @@
     <row r="153" spans="1:8">
       <c r="A153" s="7"/>
       <c r="B153" s="7"/>
-      <c r="C153" s="7"/>
+      <c r="C153" s="4"/>
       <c r="D153" s="7"/>
       <c r="E153" s="7"/>
       <c r="F153" s="7"/>
@@ -6555,7 +6627,7 @@
     </row>
     <row r="154" spans="1:8">
       <c r="A154" s="7"/>
-      <c r="B154" s="22"/>
+      <c r="B154" s="7"/>
       <c r="C154" s="7"/>
       <c r="D154" s="7"/>
       <c r="E154" s="7"/>
@@ -6575,7 +6647,7 @@
     </row>
     <row r="156" spans="1:8">
       <c r="A156" s="7"/>
-      <c r="B156" s="7"/>
+      <c r="B156" s="22"/>
       <c r="C156" s="7"/>
       <c r="D156" s="7"/>
       <c r="E156" s="7"/>
@@ -6585,7 +6657,7 @@
     </row>
     <row r="157" spans="1:8">
       <c r="A157" s="7"/>
-      <c r="B157" s="20"/>
+      <c r="B157" s="7"/>
       <c r="C157" s="7"/>
       <c r="D157" s="7"/>
       <c r="E157" s="7"/>
@@ -6605,7 +6677,7 @@
     </row>
     <row r="159" spans="1:8">
       <c r="A159" s="7"/>
-      <c r="B159" s="7"/>
+      <c r="B159" s="20"/>
       <c r="C159" s="7"/>
       <c r="D159" s="7"/>
       <c r="E159" s="7"/>
@@ -6625,7 +6697,7 @@
     </row>
     <row r="161" spans="1:8">
       <c r="A161" s="7"/>
-      <c r="B161" s="20"/>
+      <c r="B161" s="7"/>
       <c r="C161" s="7"/>
       <c r="D161" s="7"/>
       <c r="E161" s="7"/>
@@ -6645,7 +6717,7 @@
     </row>
     <row r="163" spans="1:8">
       <c r="A163" s="7"/>
-      <c r="B163" s="7"/>
+      <c r="B163" s="20"/>
       <c r="C163" s="7"/>
       <c r="D163" s="7"/>
       <c r="E163" s="7"/>
@@ -6665,7 +6737,7 @@
     </row>
     <row r="165" spans="1:8">
       <c r="A165" s="7"/>
-      <c r="B165" s="20"/>
+      <c r="B165" s="7"/>
       <c r="C165" s="7"/>
       <c r="D165" s="7"/>
       <c r="E165" s="7"/>
@@ -6685,7 +6757,7 @@
     </row>
     <row r="167" spans="1:8">
       <c r="A167" s="7"/>
-      <c r="B167" s="7"/>
+      <c r="B167" s="20"/>
       <c r="C167" s="7"/>
       <c r="D167" s="7"/>
       <c r="E167" s="7"/>
@@ -6725,7 +6797,7 @@
     </row>
     <row r="171" spans="1:8">
       <c r="A171" s="7"/>
-      <c r="B171" s="6"/>
+      <c r="B171" s="7"/>
       <c r="C171" s="7"/>
       <c r="D171" s="7"/>
       <c r="E171" s="7"/>
@@ -6735,8 +6807,8 @@
     </row>
     <row r="172" spans="1:8">
       <c r="A172" s="7"/>
-      <c r="B172" s="4"/>
-      <c r="C172" s="4"/>
+      <c r="B172" s="6"/>
+      <c r="C172" s="7"/>
       <c r="D172" s="7"/>
       <c r="E172" s="7"/>
       <c r="F172" s="7"/>
@@ -6745,7 +6817,7 @@
     </row>
     <row r="173" spans="1:8">
       <c r="A173" s="7"/>
-      <c r="B173" s="19"/>
+      <c r="B173" s="4"/>
       <c r="C173" s="4"/>
       <c r="D173" s="7"/>
       <c r="E173" s="7"/>
@@ -6815,7 +6887,7 @@
     </row>
     <row r="180" spans="1:8">
       <c r="A180" s="7"/>
-      <c r="B180" s="4"/>
+      <c r="B180" s="19"/>
       <c r="C180" s="4"/>
       <c r="D180" s="7"/>
       <c r="E180" s="7"/>
@@ -6825,7 +6897,7 @@
     </row>
     <row r="181" spans="1:8">
       <c r="A181" s="7"/>
-      <c r="B181" s="19"/>
+      <c r="B181" s="4"/>
       <c r="C181" s="4"/>
       <c r="D181" s="7"/>
       <c r="E181" s="7"/>
@@ -6835,7 +6907,7 @@
     </row>
     <row r="182" spans="1:8">
       <c r="A182" s="7"/>
-      <c r="B182" s="21"/>
+      <c r="B182" s="19"/>
       <c r="C182" s="4"/>
       <c r="D182" s="7"/>
       <c r="E182" s="7"/>
@@ -6855,7 +6927,7 @@
     </row>
     <row r="184" spans="1:8">
       <c r="A184" s="7"/>
-      <c r="B184" s="19"/>
+      <c r="B184" s="21"/>
       <c r="C184" s="4"/>
       <c r="D184" s="7"/>
       <c r="E184" s="7"/>
@@ -6896,7 +6968,7 @@
     <row r="188" spans="1:8">
       <c r="A188" s="7"/>
       <c r="B188" s="19"/>
-      <c r="C188" s="7"/>
+      <c r="C188" s="4"/>
       <c r="D188" s="7"/>
       <c r="E188" s="7"/>
       <c r="F188" s="7"/>
@@ -6905,7 +6977,7 @@
     </row>
     <row r="189" spans="1:8">
       <c r="A189" s="7"/>
-      <c r="B189" s="4"/>
+      <c r="B189" s="19"/>
       <c r="C189" s="7"/>
       <c r="D189" s="7"/>
       <c r="E189" s="7"/>
@@ -6925,7 +6997,7 @@
     </row>
     <row r="191" spans="1:8">
       <c r="A191" s="7"/>
-      <c r="B191" s="19"/>
+      <c r="B191" s="4"/>
       <c r="C191" s="7"/>
       <c r="D191" s="7"/>
       <c r="E191" s="7"/>
@@ -6985,7 +7057,7 @@
     </row>
     <row r="197" spans="1:8">
       <c r="A197" s="7"/>
-      <c r="B197" s="21"/>
+      <c r="B197" s="19"/>
       <c r="C197" s="7"/>
       <c r="D197" s="7"/>
       <c r="E197" s="7"/>
@@ -7025,7 +7097,7 @@
     </row>
     <row r="201" spans="1:8">
       <c r="A201" s="7"/>
-      <c r="B201" s="4"/>
+      <c r="B201" s="21"/>
       <c r="C201" s="7"/>
       <c r="D201" s="7"/>
       <c r="E201" s="7"/>
@@ -7035,7 +7107,7 @@
     </row>
     <row r="202" spans="1:8">
       <c r="A202" s="7"/>
-      <c r="B202" s="6"/>
+      <c r="B202" s="4"/>
       <c r="C202" s="7"/>
       <c r="D202" s="7"/>
       <c r="E202" s="7"/>
@@ -7045,7 +7117,7 @@
     </row>
     <row r="203" spans="1:8">
       <c r="A203" s="7"/>
-      <c r="B203" s="4"/>
+      <c r="B203" s="6"/>
       <c r="C203" s="7"/>
       <c r="D203" s="7"/>
       <c r="E203" s="7"/>
@@ -7055,7 +7127,7 @@
     </row>
     <row r="204" spans="1:8">
       <c r="A204" s="7"/>
-      <c r="B204" s="19"/>
+      <c r="B204" s="4"/>
       <c r="C204" s="7"/>
       <c r="D204" s="7"/>
       <c r="E204" s="7"/>
@@ -7105,7 +7177,7 @@
     </row>
     <row r="209" spans="1:8">
       <c r="A209" s="7"/>
-      <c r="B209" s="21"/>
+      <c r="B209" s="19"/>
       <c r="C209" s="7"/>
       <c r="D209" s="7"/>
       <c r="E209" s="7"/>
@@ -7115,7 +7187,7 @@
     </row>
     <row r="210" spans="1:8">
       <c r="A210" s="7"/>
-      <c r="B210" s="19"/>
+      <c r="B210" s="21"/>
       <c r="C210" s="7"/>
       <c r="D210" s="7"/>
       <c r="E210" s="7"/>
@@ -7165,7 +7237,7 @@
     </row>
     <row r="215" spans="1:8">
       <c r="A215" s="7"/>
-      <c r="B215" s="21"/>
+      <c r="B215" s="19"/>
       <c r="C215" s="7"/>
       <c r="D215" s="7"/>
       <c r="E215" s="7"/>
@@ -7225,7 +7297,7 @@
     </row>
     <row r="221" spans="1:8">
       <c r="A221" s="7"/>
-      <c r="B221" s="4"/>
+      <c r="B221" s="21"/>
       <c r="C221" s="7"/>
       <c r="D221" s="7"/>
       <c r="E221" s="7"/>
@@ -7235,7 +7307,7 @@
     </row>
     <row r="222" spans="1:8">
       <c r="A222" s="7"/>
-      <c r="B222" s="6"/>
+      <c r="B222" s="4"/>
       <c r="C222" s="7"/>
       <c r="D222" s="7"/>
       <c r="E222" s="7"/>
@@ -7245,8 +7317,8 @@
     </row>
     <row r="223" spans="1:8">
       <c r="A223" s="7"/>
-      <c r="B223" s="4"/>
-      <c r="C223" s="4"/>
+      <c r="B223" s="6"/>
+      <c r="C223" s="7"/>
       <c r="D223" s="7"/>
       <c r="E223" s="7"/>
       <c r="F223" s="7"/>
@@ -7255,7 +7327,7 @@
     </row>
     <row r="224" spans="1:8">
       <c r="A224" s="7"/>
-      <c r="B224" s="19"/>
+      <c r="B224" s="4"/>
       <c r="C224" s="4"/>
       <c r="D224" s="7"/>
       <c r="E224" s="7"/>
@@ -7265,7 +7337,7 @@
     </row>
     <row r="225" spans="1:8">
       <c r="A225" s="7"/>
-      <c r="B225" s="7"/>
+      <c r="B225" s="19"/>
       <c r="C225" s="4"/>
       <c r="D225" s="7"/>
       <c r="E225" s="7"/>
@@ -7275,7 +7347,7 @@
     </row>
     <row r="226" spans="1:8">
       <c r="A226" s="7"/>
-      <c r="B226" s="20"/>
+      <c r="B226" s="7"/>
       <c r="C226" s="4"/>
       <c r="D226" s="7"/>
       <c r="E226" s="7"/>
@@ -7315,7 +7387,7 @@
     </row>
     <row r="230" spans="1:8">
       <c r="A230" s="7"/>
-      <c r="B230" s="7"/>
+      <c r="B230" s="20"/>
       <c r="C230" s="4"/>
       <c r="D230" s="7"/>
       <c r="E230" s="7"/>
@@ -7325,7 +7397,7 @@
     </row>
     <row r="231" spans="1:8">
       <c r="A231" s="7"/>
-      <c r="B231" s="20"/>
+      <c r="B231" s="7"/>
       <c r="C231" s="4"/>
       <c r="D231" s="7"/>
       <c r="E231" s="7"/>
@@ -7335,7 +7407,7 @@
     </row>
     <row r="232" spans="1:8">
       <c r="A232" s="7"/>
-      <c r="B232" s="23"/>
+      <c r="B232" s="20"/>
       <c r="C232" s="4"/>
       <c r="D232" s="7"/>
       <c r="E232" s="7"/>
@@ -7355,7 +7427,7 @@
     </row>
     <row r="234" spans="1:8">
       <c r="A234" s="7"/>
-      <c r="B234" s="20"/>
+      <c r="B234" s="23"/>
       <c r="C234" s="4"/>
       <c r="D234" s="7"/>
       <c r="E234" s="7"/>
@@ -7395,7 +7467,7 @@
     </row>
     <row r="238" spans="1:8">
       <c r="A238" s="7"/>
-      <c r="B238" s="7"/>
+      <c r="B238" s="20"/>
       <c r="C238" s="4"/>
       <c r="D238" s="7"/>
       <c r="E238" s="7"/>
@@ -7405,7 +7477,7 @@
     </row>
     <row r="239" spans="1:8">
       <c r="A239" s="7"/>
-      <c r="B239" s="20"/>
+      <c r="B239" s="7"/>
       <c r="C239" s="4"/>
       <c r="D239" s="7"/>
       <c r="E239" s="7"/>
@@ -7455,7 +7527,7 @@
     </row>
     <row r="244" spans="1:8">
       <c r="A244" s="7"/>
-      <c r="B244" s="7"/>
+      <c r="B244" s="20"/>
       <c r="C244" s="4"/>
       <c r="D244" s="7"/>
       <c r="E244" s="7"/>
@@ -7465,8 +7537,8 @@
     </row>
     <row r="245" spans="1:8">
       <c r="A245" s="7"/>
-      <c r="B245" s="20"/>
-      <c r="C245" s="7"/>
+      <c r="B245" s="7"/>
+      <c r="C245" s="4"/>
       <c r="D245" s="7"/>
       <c r="E245" s="7"/>
       <c r="F245" s="7"/>
@@ -7475,7 +7547,7 @@
     </row>
     <row r="246" spans="1:8">
       <c r="A246" s="7"/>
-      <c r="B246" s="7"/>
+      <c r="B246" s="20"/>
       <c r="C246" s="7"/>
       <c r="D246" s="7"/>
       <c r="E246" s="7"/>
@@ -7485,7 +7557,7 @@
     </row>
     <row r="247" spans="1:8">
       <c r="A247" s="7"/>
-      <c r="B247" s="20"/>
+      <c r="B247" s="7"/>
       <c r="C247" s="7"/>
       <c r="D247" s="7"/>
       <c r="E247" s="7"/>
@@ -7495,7 +7567,7 @@
     </row>
     <row r="248" spans="1:8">
       <c r="A248" s="7"/>
-      <c r="B248" s="23"/>
+      <c r="B248" s="20"/>
       <c r="C248" s="7"/>
       <c r="D248" s="7"/>
       <c r="E248" s="7"/>
@@ -7545,8 +7617,8 @@
     </row>
     <row r="253" spans="1:8">
       <c r="A253" s="7"/>
-      <c r="B253" s="20"/>
-      <c r="C253" s="4"/>
+      <c r="B253" s="23"/>
+      <c r="C253" s="7"/>
       <c r="D253" s="7"/>
       <c r="E253" s="7"/>
       <c r="F253" s="7"/>
@@ -7555,7 +7627,7 @@
     </row>
     <row r="254" spans="1:8">
       <c r="A254" s="7"/>
-      <c r="B254" s="23"/>
+      <c r="B254" s="20"/>
       <c r="C254" s="4"/>
       <c r="D254" s="7"/>
       <c r="E254" s="7"/>
@@ -7565,7 +7637,7 @@
     </row>
     <row r="255" spans="1:8">
       <c r="A255" s="7"/>
-      <c r="B255" s="24"/>
+      <c r="B255" s="23"/>
       <c r="C255" s="4"/>
       <c r="D255" s="7"/>
       <c r="E255" s="7"/>
@@ -7593,9 +7665,9 @@
       <c r="G257" s="30"/>
       <c r="H257" s="7"/>
     </row>
-    <row r="258" spans="1:8" ht="11.25">
+    <row r="258" spans="1:8">
       <c r="A258" s="7"/>
-      <c r="B258" s="25"/>
+      <c r="B258" s="24"/>
       <c r="C258" s="4"/>
       <c r="D258" s="7"/>
       <c r="E258" s="7"/>
@@ -7603,9 +7675,9 @@
       <c r="G258" s="30"/>
       <c r="H258" s="7"/>
     </row>
-    <row r="259" spans="1:8">
+    <row r="259" spans="1:8" ht="11.25">
       <c r="A259" s="7"/>
-      <c r="B259" s="23"/>
+      <c r="B259" s="25"/>
       <c r="C259" s="4"/>
       <c r="D259" s="7"/>
       <c r="E259" s="7"/>
@@ -7645,7 +7717,7 @@
     </row>
     <row r="263" spans="1:8">
       <c r="A263" s="7"/>
-      <c r="B263" s="24"/>
+      <c r="B263" s="23"/>
       <c r="C263" s="4"/>
       <c r="D263" s="7"/>
       <c r="E263" s="7"/>
@@ -7675,7 +7747,7 @@
     </row>
     <row r="266" spans="1:8">
       <c r="A266" s="7"/>
-      <c r="B266" s="23"/>
+      <c r="B266" s="24"/>
       <c r="C266" s="4"/>
       <c r="D266" s="7"/>
       <c r="E266" s="7"/>
@@ -7685,7 +7757,7 @@
     </row>
     <row r="267" spans="1:8">
       <c r="A267" s="7"/>
-      <c r="B267" s="24"/>
+      <c r="B267" s="23"/>
       <c r="C267" s="4"/>
       <c r="D267" s="7"/>
       <c r="E267" s="7"/>
@@ -7693,15 +7765,15 @@
       <c r="G267" s="30"/>
       <c r="H267" s="7"/>
     </row>
-    <row r="268" spans="1:8" s="2" customFormat="1">
-      <c r="A268" s="4"/>
+    <row r="268" spans="1:8">
+      <c r="A268" s="7"/>
       <c r="B268" s="24"/>
       <c r="C268" s="4"/>
-      <c r="D268" s="4"/>
-      <c r="E268" s="4"/>
-      <c r="F268" s="4"/>
-      <c r="G268" s="34"/>
-      <c r="H268" s="4"/>
+      <c r="D268" s="7"/>
+      <c r="E268" s="7"/>
+      <c r="F268" s="7"/>
+      <c r="G268" s="30"/>
+      <c r="H268" s="7"/>
     </row>
     <row r="269" spans="1:8" s="2" customFormat="1">
       <c r="A269" s="4"/>
@@ -7713,19 +7785,19 @@
       <c r="G269" s="34"/>
       <c r="H269" s="4"/>
     </row>
-    <row r="270" spans="1:8">
-      <c r="A270" s="7"/>
+    <row r="270" spans="1:8" s="2" customFormat="1">
+      <c r="A270" s="4"/>
       <c r="B270" s="24"/>
       <c r="C270" s="4"/>
-      <c r="D270" s="7"/>
-      <c r="E270" s="7"/>
-      <c r="F270" s="7"/>
-      <c r="G270" s="30"/>
-      <c r="H270" s="7"/>
+      <c r="D270" s="4"/>
+      <c r="E270" s="4"/>
+      <c r="F270" s="4"/>
+      <c r="G270" s="34"/>
+      <c r="H270" s="4"/>
     </row>
     <row r="271" spans="1:8">
       <c r="A271" s="7"/>
-      <c r="B271" s="23"/>
+      <c r="B271" s="24"/>
       <c r="C271" s="4"/>
       <c r="D271" s="7"/>
       <c r="E271" s="7"/>
@@ -7735,7 +7807,7 @@
     </row>
     <row r="272" spans="1:8">
       <c r="A272" s="7"/>
-      <c r="B272" s="24"/>
+      <c r="B272" s="23"/>
       <c r="C272" s="4"/>
       <c r="D272" s="7"/>
       <c r="E272" s="7"/>
@@ -7765,7 +7837,7 @@
     </row>
     <row r="275" spans="1:8">
       <c r="A275" s="7"/>
-      <c r="B275" s="22"/>
+      <c r="B275" s="24"/>
       <c r="C275" s="4"/>
       <c r="D275" s="7"/>
       <c r="E275" s="7"/>
@@ -7775,7 +7847,7 @@
     </row>
     <row r="276" spans="1:8">
       <c r="A276" s="7"/>
-      <c r="B276" s="7"/>
+      <c r="B276" s="22"/>
       <c r="C276" s="4"/>
       <c r="D276" s="7"/>
       <c r="E276" s="7"/>
@@ -7795,7 +7867,7 @@
     </row>
     <row r="278" spans="1:8">
       <c r="A278" s="7"/>
-      <c r="B278" s="20"/>
+      <c r="B278" s="7"/>
       <c r="C278" s="4"/>
       <c r="D278" s="7"/>
       <c r="E278" s="7"/>
@@ -7815,7 +7887,7 @@
     </row>
     <row r="280" spans="1:8">
       <c r="A280" s="7"/>
-      <c r="B280" s="7"/>
+      <c r="B280" s="20"/>
       <c r="C280" s="4"/>
       <c r="D280" s="7"/>
       <c r="E280" s="7"/>
@@ -7846,7 +7918,7 @@
     <row r="283" spans="1:8">
       <c r="A283" s="7"/>
       <c r="B283" s="7"/>
-      <c r="C283" s="7"/>
+      <c r="C283" s="4"/>
       <c r="D283" s="7"/>
       <c r="E283" s="7"/>
       <c r="F283" s="7"/>
@@ -7855,7 +7927,7 @@
     </row>
     <row r="284" spans="1:8">
       <c r="A284" s="7"/>
-      <c r="B284" s="6"/>
+      <c r="B284" s="7"/>
       <c r="C284" s="7"/>
       <c r="D284" s="7"/>
       <c r="E284" s="7"/>
@@ -7865,7 +7937,7 @@
     </row>
     <row r="285" spans="1:8">
       <c r="A285" s="7"/>
-      <c r="B285" s="7"/>
+      <c r="B285" s="6"/>
       <c r="C285" s="7"/>
       <c r="D285" s="7"/>
       <c r="E285" s="7"/>
@@ -7945,7 +8017,7 @@
     </row>
     <row r="293" spans="1:8">
       <c r="A293" s="7"/>
-      <c r="B293" s="6"/>
+      <c r="B293" s="7"/>
       <c r="C293" s="7"/>
       <c r="D293" s="7"/>
       <c r="E293" s="7"/>
@@ -7955,8 +8027,8 @@
     </row>
     <row r="294" spans="1:8">
       <c r="A294" s="7"/>
-      <c r="B294" s="4"/>
-      <c r="C294" s="4"/>
+      <c r="B294" s="6"/>
+      <c r="C294" s="7"/>
       <c r="D294" s="7"/>
       <c r="E294" s="7"/>
       <c r="F294" s="7"/>
@@ -7965,7 +8037,7 @@
     </row>
     <row r="295" spans="1:8">
       <c r="A295" s="7"/>
-      <c r="B295" s="19"/>
+      <c r="B295" s="4"/>
       <c r="C295" s="4"/>
       <c r="D295" s="7"/>
       <c r="E295" s="7"/>
@@ -7995,7 +8067,7 @@
     </row>
     <row r="298" spans="1:8">
       <c r="A298" s="7"/>
-      <c r="B298" s="4"/>
+      <c r="B298" s="19"/>
       <c r="C298" s="4"/>
       <c r="D298" s="7"/>
       <c r="E298" s="7"/>
@@ -8055,7 +8127,7 @@
     </row>
     <row r="304" spans="1:8">
       <c r="A304" s="7"/>
-      <c r="B304" s="19"/>
+      <c r="B304" s="4"/>
       <c r="C304" s="4"/>
       <c r="D304" s="7"/>
       <c r="E304" s="7"/>
@@ -8075,7 +8147,7 @@
     </row>
     <row r="306" spans="1:8">
       <c r="A306" s="7"/>
-      <c r="B306" s="21"/>
+      <c r="B306" s="19"/>
       <c r="C306" s="4"/>
       <c r="D306" s="7"/>
       <c r="E306" s="7"/>
@@ -8085,8 +8157,8 @@
     </row>
     <row r="307" spans="1:8">
       <c r="A307" s="7"/>
-      <c r="B307" s="7"/>
-      <c r="C307" s="7"/>
+      <c r="B307" s="21"/>
+      <c r="C307" s="4"/>
       <c r="D307" s="7"/>
       <c r="E307" s="7"/>
       <c r="F307" s="7"/>
@@ -8095,7 +8167,7 @@
     </row>
     <row r="308" spans="1:8">
       <c r="A308" s="7"/>
-      <c r="B308" s="6"/>
+      <c r="B308" s="7"/>
       <c r="C308" s="7"/>
       <c r="D308" s="7"/>
       <c r="E308" s="7"/>
@@ -8103,15 +8175,15 @@
       <c r="G308" s="30"/>
       <c r="H308" s="7"/>
     </row>
-    <row r="309" spans="1:8" s="2" customFormat="1">
-      <c r="A309" s="4"/>
-      <c r="B309" s="4"/>
-      <c r="C309" s="9"/>
-      <c r="D309" s="4"/>
-      <c r="E309" s="4"/>
-      <c r="F309" s="4"/>
-      <c r="G309" s="34"/>
-      <c r="H309" s="4"/>
+    <row r="309" spans="1:8">
+      <c r="A309" s="7"/>
+      <c r="B309" s="6"/>
+      <c r="C309" s="7"/>
+      <c r="D309" s="7"/>
+      <c r="E309" s="7"/>
+      <c r="F309" s="7"/>
+      <c r="G309" s="30"/>
+      <c r="H309" s="7"/>
     </row>
     <row r="310" spans="1:8" s="2" customFormat="1">
       <c r="A310" s="4"/>
@@ -8135,7 +8207,7 @@
     </row>
     <row r="312" spans="1:8" s="2" customFormat="1">
       <c r="A312" s="4"/>
-      <c r="B312" s="19"/>
+      <c r="B312" s="4"/>
       <c r="C312" s="9"/>
       <c r="D312" s="4"/>
       <c r="E312" s="4"/>
@@ -8185,8 +8257,8 @@
     </row>
     <row r="317" spans="1:8" s="2" customFormat="1">
       <c r="A317" s="4"/>
-      <c r="B317" s="26"/>
-      <c r="C317" s="4"/>
+      <c r="B317" s="19"/>
+      <c r="C317" s="9"/>
       <c r="D317" s="4"/>
       <c r="E317" s="4"/>
       <c r="F317" s="4"/>
@@ -8235,7 +8307,7 @@
     </row>
     <row r="322" spans="1:8" s="2" customFormat="1">
       <c r="A322" s="4"/>
-      <c r="B322" s="21"/>
+      <c r="B322" s="26"/>
       <c r="C322" s="4"/>
       <c r="D322" s="4"/>
       <c r="E322" s="4"/>
@@ -8285,7 +8357,7 @@
     </row>
     <row r="327" spans="1:8" s="2" customFormat="1">
       <c r="A327" s="4"/>
-      <c r="B327" s="19"/>
+      <c r="B327" s="21"/>
       <c r="C327" s="4"/>
       <c r="D327" s="4"/>
       <c r="E327" s="4"/>
@@ -8295,7 +8367,7 @@
     </row>
     <row r="328" spans="1:8" s="2" customFormat="1">
       <c r="A328" s="4"/>
-      <c r="B328" s="21"/>
+      <c r="B328" s="19"/>
       <c r="C328" s="4"/>
       <c r="D328" s="4"/>
       <c r="E328" s="4"/>
@@ -8305,7 +8377,7 @@
     </row>
     <row r="329" spans="1:8" s="2" customFormat="1">
       <c r="A329" s="4"/>
-      <c r="B329" s="4"/>
+      <c r="B329" s="21"/>
       <c r="C329" s="4"/>
       <c r="D329" s="4"/>
       <c r="E329" s="4"/>
@@ -8313,20 +8385,20 @@
       <c r="G329" s="34"/>
       <c r="H329" s="4"/>
     </row>
-    <row r="330" spans="1:8">
-      <c r="A330" s="7"/>
-      <c r="B330" s="6"/>
-      <c r="C330" s="7"/>
-      <c r="D330" s="7"/>
-      <c r="E330" s="7"/>
-      <c r="F330" s="7"/>
-      <c r="G330" s="30"/>
-      <c r="H330" s="7"/>
+    <row r="330" spans="1:8" s="2" customFormat="1">
+      <c r="A330" s="4"/>
+      <c r="B330" s="4"/>
+      <c r="C330" s="4"/>
+      <c r="D330" s="4"/>
+      <c r="E330" s="4"/>
+      <c r="F330" s="4"/>
+      <c r="G330" s="34"/>
+      <c r="H330" s="4"/>
     </row>
     <row r="331" spans="1:8">
       <c r="A331" s="7"/>
-      <c r="B331" s="7"/>
-      <c r="C331" s="4"/>
+      <c r="B331" s="6"/>
+      <c r="C331" s="7"/>
       <c r="D331" s="7"/>
       <c r="E331" s="7"/>
       <c r="F331" s="7"/>
@@ -8395,7 +8467,7 @@
     </row>
     <row r="338" spans="1:8">
       <c r="A338" s="7"/>
-      <c r="B338" s="4"/>
+      <c r="B338" s="7"/>
       <c r="C338" s="4"/>
       <c r="D338" s="7"/>
       <c r="E338" s="7"/>
@@ -8406,7 +8478,7 @@
     <row r="339" spans="1:8">
       <c r="A339" s="7"/>
       <c r="B339" s="4"/>
-      <c r="C339" s="7"/>
+      <c r="C339" s="4"/>
       <c r="D339" s="7"/>
       <c r="E339" s="7"/>
       <c r="F339" s="7"/>
@@ -8415,7 +8487,7 @@
     </row>
     <row r="340" spans="1:8">
       <c r="A340" s="7"/>
-      <c r="B340" s="6"/>
+      <c r="B340" s="4"/>
       <c r="C340" s="7"/>
       <c r="D340" s="7"/>
       <c r="E340" s="7"/>
@@ -8425,7 +8497,7 @@
     </row>
     <row r="341" spans="1:8">
       <c r="A341" s="7"/>
-      <c r="B341" s="7"/>
+      <c r="B341" s="6"/>
       <c r="C341" s="7"/>
       <c r="D341" s="7"/>
       <c r="E341" s="7"/>
@@ -8435,7 +8507,7 @@
     </row>
     <row r="342" spans="1:8">
       <c r="A342" s="7"/>
-      <c r="B342" s="22"/>
+      <c r="B342" s="7"/>
       <c r="C342" s="7"/>
       <c r="D342" s="7"/>
       <c r="E342" s="7"/>
@@ -8445,7 +8517,7 @@
     </row>
     <row r="343" spans="1:8">
       <c r="A343" s="7"/>
-      <c r="B343" s="7"/>
+      <c r="B343" s="22"/>
       <c r="C343" s="7"/>
       <c r="D343" s="7"/>
       <c r="E343" s="7"/>
@@ -8485,7 +8557,7 @@
     </row>
     <row r="347" spans="1:8">
       <c r="A347" s="7"/>
-      <c r="B347" s="6"/>
+      <c r="B347" s="7"/>
       <c r="C347" s="7"/>
       <c r="D347" s="7"/>
       <c r="E347" s="7"/>
@@ -8495,7 +8567,7 @@
     </row>
     <row r="348" spans="1:8">
       <c r="A348" s="7"/>
-      <c r="B348" s="7"/>
+      <c r="B348" s="6"/>
       <c r="C348" s="7"/>
       <c r="D348" s="7"/>
       <c r="E348" s="7"/>
@@ -8505,7 +8577,7 @@
     </row>
     <row r="349" spans="1:8">
       <c r="A349" s="7"/>
-      <c r="B349" s="20"/>
+      <c r="B349" s="7"/>
       <c r="C349" s="7"/>
       <c r="D349" s="7"/>
       <c r="E349" s="7"/>
@@ -8535,7 +8607,7 @@
     </row>
     <row r="352" spans="1:8">
       <c r="A352" s="7"/>
-      <c r="B352" s="22"/>
+      <c r="B352" s="20"/>
       <c r="C352" s="7"/>
       <c r="D352" s="7"/>
       <c r="E352" s="7"/>
@@ -8545,7 +8617,7 @@
     </row>
     <row r="353" spans="1:8">
       <c r="A353" s="7"/>
-      <c r="B353" s="20"/>
+      <c r="B353" s="22"/>
       <c r="C353" s="7"/>
       <c r="D353" s="7"/>
       <c r="E353" s="7"/>
@@ -8565,7 +8637,7 @@
     </row>
     <row r="355" spans="1:8">
       <c r="A355" s="7"/>
-      <c r="B355" s="22"/>
+      <c r="B355" s="20"/>
       <c r="C355" s="7"/>
       <c r="D355" s="7"/>
       <c r="E355" s="7"/>
@@ -8575,7 +8647,7 @@
     </row>
     <row r="356" spans="1:8">
       <c r="A356" s="7"/>
-      <c r="B356" s="20"/>
+      <c r="B356" s="22"/>
       <c r="C356" s="7"/>
       <c r="D356" s="7"/>
       <c r="E356" s="7"/>
@@ -8585,7 +8657,7 @@
     </row>
     <row r="357" spans="1:8">
       <c r="A357" s="7"/>
-      <c r="B357" s="22"/>
+      <c r="B357" s="20"/>
       <c r="C357" s="7"/>
       <c r="D357" s="7"/>
       <c r="E357" s="7"/>
@@ -8595,7 +8667,7 @@
     </row>
     <row r="358" spans="1:8">
       <c r="A358" s="7"/>
-      <c r="B358" s="20"/>
+      <c r="B358" s="22"/>
       <c r="C358" s="7"/>
       <c r="D358" s="7"/>
       <c r="E358" s="7"/>
@@ -8625,7 +8697,7 @@
     </row>
     <row r="361" spans="1:8">
       <c r="A361" s="7"/>
-      <c r="B361" s="7"/>
+      <c r="B361" s="20"/>
       <c r="C361" s="7"/>
       <c r="D361" s="7"/>
       <c r="E361" s="7"/>
@@ -8635,7 +8707,7 @@
     </row>
     <row r="362" spans="1:8">
       <c r="A362" s="7"/>
-      <c r="B362" s="27"/>
+      <c r="B362" s="7"/>
       <c r="C362" s="7"/>
       <c r="D362" s="7"/>
       <c r="E362" s="7"/>
@@ -8645,7 +8717,7 @@
     </row>
     <row r="363" spans="1:8">
       <c r="A363" s="7"/>
-      <c r="B363" s="22"/>
+      <c r="B363" s="27"/>
       <c r="C363" s="7"/>
       <c r="D363" s="7"/>
       <c r="E363" s="7"/>
@@ -8655,8 +8727,8 @@
     </row>
     <row r="364" spans="1:8">
       <c r="A364" s="7"/>
-      <c r="B364" s="7"/>
-      <c r="C364" s="4"/>
+      <c r="B364" s="22"/>
+      <c r="C364" s="7"/>
       <c r="D364" s="7"/>
       <c r="E364" s="7"/>
       <c r="F364" s="7"/>
@@ -8665,7 +8737,7 @@
     </row>
     <row r="365" spans="1:8">
       <c r="A365" s="7"/>
-      <c r="B365" s="20"/>
+      <c r="B365" s="7"/>
       <c r="C365" s="4"/>
       <c r="D365" s="7"/>
       <c r="E365" s="7"/>
@@ -8695,7 +8767,7 @@
     </row>
     <row r="368" spans="1:8">
       <c r="A368" s="7"/>
-      <c r="B368" s="7"/>
+      <c r="B368" s="20"/>
       <c r="C368" s="4"/>
       <c r="D368" s="7"/>
       <c r="E368" s="7"/>
@@ -8725,7 +8797,7 @@
     </row>
     <row r="371" spans="1:8">
       <c r="A371" s="7"/>
-      <c r="B371" s="20"/>
+      <c r="B371" s="7"/>
       <c r="C371" s="4"/>
       <c r="D371" s="7"/>
       <c r="E371" s="7"/>
@@ -8745,8 +8817,8 @@
     </row>
     <row r="373" spans="1:8">
       <c r="A373" s="7"/>
-      <c r="B373" s="7"/>
-      <c r="C373" s="7"/>
+      <c r="B373" s="20"/>
+      <c r="C373" s="4"/>
       <c r="D373" s="7"/>
       <c r="E373" s="7"/>
       <c r="F373" s="7"/>
@@ -8755,7 +8827,7 @@
     </row>
     <row r="374" spans="1:8">
       <c r="A374" s="7"/>
-      <c r="B374" s="6"/>
+      <c r="B374" s="7"/>
       <c r="C374" s="7"/>
       <c r="D374" s="7"/>
       <c r="E374" s="7"/>
@@ -8765,7 +8837,7 @@
     </row>
     <row r="375" spans="1:8">
       <c r="A375" s="7"/>
-      <c r="B375" s="7"/>
+      <c r="B375" s="6"/>
       <c r="C375" s="7"/>
       <c r="D375" s="7"/>
       <c r="E375" s="7"/>
@@ -8825,7 +8897,7 @@
     </row>
     <row r="381" spans="1:8">
       <c r="A381" s="7"/>
-      <c r="B381" s="6"/>
+      <c r="B381" s="7"/>
       <c r="C381" s="7"/>
       <c r="D381" s="7"/>
       <c r="E381" s="7"/>
@@ -8835,7 +8907,7 @@
     </row>
     <row r="382" spans="1:8">
       <c r="A382" s="7"/>
-      <c r="B382" s="7"/>
+      <c r="B382" s="6"/>
       <c r="C382" s="7"/>
       <c r="D382" s="7"/>
       <c r="E382" s="7"/>
@@ -8856,7 +8928,7 @@
     <row r="384" spans="1:8">
       <c r="A384" s="7"/>
       <c r="B384" s="7"/>
-      <c r="C384" s="4"/>
+      <c r="C384" s="7"/>
       <c r="D384" s="7"/>
       <c r="E384" s="7"/>
       <c r="F384" s="7"/>
@@ -8865,7 +8937,7 @@
     </row>
     <row r="385" spans="1:8">
       <c r="A385" s="7"/>
-      <c r="B385" s="20"/>
+      <c r="B385" s="7"/>
       <c r="C385" s="4"/>
       <c r="D385" s="7"/>
       <c r="E385" s="7"/>
@@ -8876,7 +8948,7 @@
     <row r="386" spans="1:8">
       <c r="A386" s="7"/>
       <c r="B386" s="20"/>
-      <c r="C386" s="7"/>
+      <c r="C386" s="4"/>
       <c r="D386" s="7"/>
       <c r="E386" s="7"/>
       <c r="F386" s="7"/>
@@ -8885,7 +8957,7 @@
     </row>
     <row r="387" spans="1:8">
       <c r="A387" s="7"/>
-      <c r="B387" s="27"/>
+      <c r="B387" s="20"/>
       <c r="C387" s="7"/>
       <c r="D387" s="7"/>
       <c r="E387" s="7"/>
@@ -8895,7 +8967,7 @@
     </row>
     <row r="388" spans="1:8">
       <c r="A388" s="7"/>
-      <c r="B388" s="22"/>
+      <c r="B388" s="27"/>
       <c r="C388" s="7"/>
       <c r="D388" s="7"/>
       <c r="E388" s="7"/>
@@ -8945,7 +9017,7 @@
     </row>
     <row r="393" spans="1:8">
       <c r="A393" s="7"/>
-      <c r="B393" s="7"/>
+      <c r="B393" s="22"/>
       <c r="C393" s="7"/>
       <c r="D393" s="7"/>
       <c r="E393" s="7"/>
@@ -8955,7 +9027,7 @@
     </row>
     <row r="394" spans="1:8">
       <c r="A394" s="7"/>
-      <c r="B394" s="6"/>
+      <c r="B394" s="7"/>
       <c r="C394" s="7"/>
       <c r="D394" s="7"/>
       <c r="E394" s="7"/>
@@ -8965,7 +9037,7 @@
     </row>
     <row r="395" spans="1:8">
       <c r="A395" s="7"/>
-      <c r="B395" s="7"/>
+      <c r="B395" s="6"/>
       <c r="C395" s="7"/>
       <c r="D395" s="7"/>
       <c r="E395" s="7"/>
@@ -8975,7 +9047,7 @@
     </row>
     <row r="396" spans="1:8">
       <c r="A396" s="7"/>
-      <c r="B396" s="20"/>
+      <c r="B396" s="7"/>
       <c r="C396" s="7"/>
       <c r="D396" s="7"/>
       <c r="E396" s="7"/>
@@ -8985,7 +9057,7 @@
     </row>
     <row r="397" spans="1:8">
       <c r="A397" s="7"/>
-      <c r="B397" s="22"/>
+      <c r="B397" s="20"/>
       <c r="C397" s="7"/>
       <c r="D397" s="7"/>
       <c r="E397" s="7"/>
@@ -9005,7 +9077,7 @@
     </row>
     <row r="399" spans="1:8">
       <c r="A399" s="7"/>
-      <c r="B399" s="20"/>
+      <c r="B399" s="22"/>
       <c r="C399" s="7"/>
       <c r="D399" s="7"/>
       <c r="E399" s="7"/>
@@ -9045,7 +9117,7 @@
     </row>
     <row r="403" spans="1:8">
       <c r="A403" s="7"/>
-      <c r="B403" s="7"/>
+      <c r="B403" s="20"/>
       <c r="C403" s="7"/>
       <c r="D403" s="7"/>
       <c r="E403" s="7"/>
@@ -9055,7 +9127,7 @@
     </row>
     <row r="404" spans="1:8">
       <c r="A404" s="7"/>
-      <c r="B404" s="20"/>
+      <c r="B404" s="7"/>
       <c r="C404" s="7"/>
       <c r="D404" s="7"/>
       <c r="E404" s="7"/>
@@ -9075,7 +9147,7 @@
     </row>
     <row r="406" spans="1:8">
       <c r="A406" s="7"/>
-      <c r="B406" s="22"/>
+      <c r="B406" s="20"/>
       <c r="C406" s="7"/>
       <c r="D406" s="7"/>
       <c r="E406" s="7"/>
@@ -9085,7 +9157,7 @@
     </row>
     <row r="407" spans="1:8">
       <c r="A407" s="7"/>
-      <c r="B407" s="7"/>
+      <c r="B407" s="22"/>
       <c r="C407" s="7"/>
       <c r="D407" s="7"/>
       <c r="E407" s="7"/>
@@ -9095,7 +9167,7 @@
     </row>
     <row r="408" spans="1:8">
       <c r="A408" s="7"/>
-      <c r="B408" s="6"/>
+      <c r="B408" s="7"/>
       <c r="C408" s="7"/>
       <c r="D408" s="7"/>
       <c r="E408" s="7"/>
@@ -9105,7 +9177,7 @@
     </row>
     <row r="409" spans="1:8">
       <c r="A409" s="7"/>
-      <c r="B409" s="7"/>
+      <c r="B409" s="6"/>
       <c r="C409" s="7"/>
       <c r="D409" s="7"/>
       <c r="E409" s="7"/>
@@ -9125,7 +9197,7 @@
     </row>
     <row r="411" spans="1:8">
       <c r="A411" s="7"/>
-      <c r="B411" s="6"/>
+      <c r="B411" s="7"/>
       <c r="C411" s="7"/>
       <c r="D411" s="7"/>
       <c r="E411" s="7"/>
@@ -9135,7 +9207,7 @@
     </row>
     <row r="412" spans="1:8">
       <c r="A412" s="7"/>
-      <c r="B412" s="7"/>
+      <c r="B412" s="6"/>
       <c r="C412" s="7"/>
       <c r="D412" s="7"/>
       <c r="E412" s="7"/>
@@ -9145,7 +9217,7 @@
     </row>
     <row r="413" spans="1:8">
       <c r="A413" s="7"/>
-      <c r="B413" s="20"/>
+      <c r="B413" s="7"/>
       <c r="C413" s="7"/>
       <c r="D413" s="7"/>
       <c r="E413" s="7"/>
@@ -9165,7 +9237,7 @@
     </row>
     <row r="415" spans="1:8">
       <c r="A415" s="7"/>
-      <c r="B415" s="7"/>
+      <c r="B415" s="20"/>
       <c r="C415" s="7"/>
       <c r="D415" s="7"/>
       <c r="E415" s="7"/>
@@ -9175,7 +9247,7 @@
     </row>
     <row r="416" spans="1:8">
       <c r="A416" s="7"/>
-      <c r="B416" s="6"/>
+      <c r="B416" s="7"/>
       <c r="C416" s="7"/>
       <c r="D416" s="7"/>
       <c r="E416" s="7"/>
@@ -9185,7 +9257,7 @@
     </row>
     <row r="417" spans="1:8">
       <c r="A417" s="7"/>
-      <c r="B417" s="7"/>
+      <c r="B417" s="6"/>
       <c r="C417" s="7"/>
       <c r="D417" s="7"/>
       <c r="E417" s="7"/>
@@ -9235,7 +9307,7 @@
     </row>
     <row r="422" spans="1:8">
       <c r="A422" s="7"/>
-      <c r="B422" s="6"/>
+      <c r="B422" s="7"/>
       <c r="C422" s="7"/>
       <c r="D422" s="7"/>
       <c r="E422" s="7"/>
@@ -9245,7 +9317,7 @@
     </row>
     <row r="423" spans="1:8">
       <c r="A423" s="7"/>
-      <c r="B423" s="7"/>
+      <c r="B423" s="6"/>
       <c r="C423" s="7"/>
       <c r="D423" s="7"/>
       <c r="E423" s="7"/>
@@ -9305,7 +9377,7 @@
     </row>
     <row r="429" spans="1:8">
       <c r="A429" s="7"/>
-      <c r="B429" s="6"/>
+      <c r="B429" s="7"/>
       <c r="C429" s="7"/>
       <c r="D429" s="7"/>
       <c r="E429" s="7"/>
@@ -9315,7 +9387,7 @@
     </row>
     <row r="430" spans="1:8">
       <c r="A430" s="7"/>
-      <c r="B430" s="7"/>
+      <c r="B430" s="6"/>
       <c r="C430" s="7"/>
       <c r="D430" s="7"/>
       <c r="E430" s="7"/>
@@ -9335,7 +9407,7 @@
     </row>
     <row r="432" spans="1:8">
       <c r="A432" s="7"/>
-      <c r="B432" s="6"/>
+      <c r="B432" s="7"/>
       <c r="C432" s="7"/>
       <c r="D432" s="7"/>
       <c r="E432" s="7"/>
@@ -9345,7 +9417,7 @@
     </row>
     <row r="433" spans="1:8">
       <c r="A433" s="7"/>
-      <c r="B433" s="4"/>
+      <c r="B433" s="6"/>
       <c r="C433" s="7"/>
       <c r="D433" s="7"/>
       <c r="E433" s="7"/>
@@ -9365,7 +9437,7 @@
     </row>
     <row r="435" spans="1:8">
       <c r="A435" s="7"/>
-      <c r="B435" s="7"/>
+      <c r="B435" s="4"/>
       <c r="C435" s="7"/>
       <c r="D435" s="7"/>
       <c r="E435" s="7"/>
@@ -9395,7 +9467,7 @@
     </row>
     <row r="438" spans="1:8">
       <c r="A438" s="7"/>
-      <c r="B438" s="6"/>
+      <c r="B438" s="7"/>
       <c r="C438" s="7"/>
       <c r="D438" s="7"/>
       <c r="E438" s="7"/>
@@ -9405,8 +9477,8 @@
     </row>
     <row r="439" spans="1:8">
       <c r="A439" s="7"/>
-      <c r="B439" s="7"/>
-      <c r="C439" s="4"/>
+      <c r="B439" s="6"/>
+      <c r="C439" s="7"/>
       <c r="D439" s="7"/>
       <c r="E439" s="7"/>
       <c r="F439" s="7"/>
@@ -9456,7 +9528,7 @@
     <row r="444" spans="1:8">
       <c r="A444" s="7"/>
       <c r="B444" s="7"/>
-      <c r="C444" s="7"/>
+      <c r="C444" s="4"/>
       <c r="D444" s="7"/>
       <c r="E444" s="7"/>
       <c r="F444" s="7"/>
@@ -9465,7 +9537,7 @@
     </row>
     <row r="445" spans="1:8">
       <c r="A445" s="7"/>
-      <c r="B445" s="6"/>
+      <c r="B445" s="7"/>
       <c r="C445" s="7"/>
       <c r="D445" s="7"/>
       <c r="E445" s="7"/>
@@ -9475,8 +9547,8 @@
     </row>
     <row r="446" spans="1:8">
       <c r="A446" s="7"/>
-      <c r="B446" s="7"/>
-      <c r="C446" s="4"/>
+      <c r="B446" s="6"/>
+      <c r="C446" s="7"/>
       <c r="D446" s="7"/>
       <c r="E446" s="7"/>
       <c r="F446" s="7"/>
@@ -9516,7 +9588,7 @@
     <row r="450" spans="1:8">
       <c r="A450" s="7"/>
       <c r="B450" s="7"/>
-      <c r="C450" s="7"/>
+      <c r="C450" s="4"/>
       <c r="D450" s="7"/>
       <c r="E450" s="7"/>
       <c r="F450" s="7"/>
@@ -9525,7 +9597,7 @@
     </row>
     <row r="451" spans="1:8">
       <c r="A451" s="7"/>
-      <c r="B451" s="6"/>
+      <c r="B451" s="7"/>
       <c r="C451" s="7"/>
       <c r="D451" s="7"/>
       <c r="E451" s="7"/>
@@ -9535,7 +9607,7 @@
     </row>
     <row r="452" spans="1:8">
       <c r="A452" s="7"/>
-      <c r="B452" s="22"/>
+      <c r="B452" s="6"/>
       <c r="C452" s="7"/>
       <c r="D452" s="7"/>
       <c r="E452" s="7"/>
@@ -9595,7 +9667,7 @@
     </row>
     <row r="458" spans="1:8">
       <c r="A458" s="7"/>
-      <c r="B458" s="7"/>
+      <c r="B458" s="22"/>
       <c r="C458" s="7"/>
       <c r="D458" s="7"/>
       <c r="E458" s="7"/>
@@ -9605,7 +9677,7 @@
     </row>
     <row r="459" spans="1:8">
       <c r="A459" s="7"/>
-      <c r="B459" s="6"/>
+      <c r="B459" s="7"/>
       <c r="C459" s="7"/>
       <c r="D459" s="7"/>
       <c r="E459" s="7"/>
@@ -9615,7 +9687,7 @@
     </row>
     <row r="460" spans="1:8">
       <c r="A460" s="7"/>
-      <c r="B460" s="22"/>
+      <c r="B460" s="6"/>
       <c r="C460" s="7"/>
       <c r="D460" s="7"/>
       <c r="E460" s="7"/>
@@ -9644,8 +9716,8 @@
       <c r="H462" s="7"/>
     </row>
     <row r="463" spans="1:8">
-      <c r="A463" s="6"/>
-      <c r="B463" s="7"/>
+      <c r="A463" s="7"/>
+      <c r="B463" s="22"/>
       <c r="C463" s="7"/>
       <c r="D463" s="7"/>
       <c r="E463" s="7"/>
@@ -9654,7 +9726,7 @@
       <c r="H463" s="7"/>
     </row>
     <row r="464" spans="1:8">
-      <c r="A464" s="7"/>
+      <c r="A464" s="6"/>
       <c r="B464" s="7"/>
       <c r="C464" s="7"/>
       <c r="D464" s="7"/>
@@ -9695,7 +9767,7 @@
     </row>
     <row r="468" spans="1:8">
       <c r="A468" s="7"/>
-      <c r="B468" s="28"/>
+      <c r="B468" s="7"/>
       <c r="C468" s="7"/>
       <c r="D468" s="7"/>
       <c r="E468" s="7"/>
@@ -9725,7 +9797,7 @@
     </row>
     <row r="471" spans="1:8">
       <c r="A471" s="7"/>
-      <c r="B471" s="7"/>
+      <c r="B471" s="28"/>
       <c r="C471" s="7"/>
       <c r="D471" s="7"/>
       <c r="E471" s="7"/>
@@ -9735,7 +9807,7 @@
     </row>
     <row r="472" spans="1:8">
       <c r="A472" s="7"/>
-      <c r="B472" s="28"/>
+      <c r="B472" s="7"/>
       <c r="C472" s="7"/>
       <c r="D472" s="7"/>
       <c r="E472" s="7"/>
@@ -9745,7 +9817,7 @@
     </row>
     <row r="473" spans="1:8">
       <c r="A473" s="7"/>
-      <c r="B473" s="7"/>
+      <c r="B473" s="28"/>
       <c r="C473" s="7"/>
       <c r="D473" s="7"/>
       <c r="E473" s="7"/>
@@ -9755,21 +9827,21 @@
     </row>
     <row r="474" spans="1:8">
       <c r="A474" s="7"/>
-      <c r="B474" s="29"/>
-      <c r="C474" s="30"/>
+      <c r="B474" s="7"/>
+      <c r="C474" s="7"/>
       <c r="D474" s="7"/>
       <c r="E474" s="7"/>
-      <c r="F474" s="29"/>
+      <c r="F474" s="7"/>
       <c r="G474" s="30"/>
       <c r="H474" s="7"/>
     </row>
     <row r="475" spans="1:8">
       <c r="A475" s="7"/>
-      <c r="B475" s="7"/>
-      <c r="C475" s="7"/>
+      <c r="B475" s="29"/>
+      <c r="C475" s="30"/>
       <c r="D475" s="7"/>
       <c r="E475" s="7"/>
-      <c r="F475" s="7"/>
+      <c r="F475" s="29"/>
       <c r="G475" s="30"/>
       <c r="H475" s="7"/>
     </row>
@@ -13673,6 +13745,16 @@
       <c r="G865" s="30"/>
       <c r="H865" s="7"/>
     </row>
+    <row r="866" spans="1:8">
+      <c r="A866" s="7"/>
+      <c r="B866" s="7"/>
+      <c r="C866" s="7"/>
+      <c r="D866" s="7"/>
+      <c r="E866" s="7"/>
+      <c r="F866" s="7"/>
+      <c r="G866" s="30"/>
+      <c r="H866" s="7"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>